<commit_message>
swicthes to guide's daily
</commit_message>
<xml_diff>
--- a/data/indicators_input.xlsx
+++ b/data/indicators_input.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="168">
   <si>
     <t>Index</t>
   </si>
@@ -314,7 +314,7 @@
     <t>DV01 -  126 Bus. Days Average</t>
   </si>
   <si>
-    <t>Overall market</t>
+    <t>Markeit</t>
   </si>
   <si>
     <t>V17</t>
@@ -470,19 +470,28 @@
     <t>Impact</t>
   </si>
   <si>
-    <t>US</t>
-  </si>
-  <si>
-    <t>Factory Orders</t>
-  </si>
-  <si>
-    <t>July</t>
-  </si>
-  <si>
-    <t>-3,3% mom</t>
+    <t>BZ</t>
+  </si>
+  <si>
+    <t>IGP-M 1F @ 0,345</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>0,34% mom</t>
   </si>
   <si>
     <t>Medium</t>
+  </si>
+  <si>
+    <t>IPC-S @ 0,10%</t>
+  </si>
+  <si>
+    <t>1W Sep</t>
+  </si>
+  <si>
+    <t>0,10% mom</t>
   </si>
   <si>
     <t>Contract</t>
@@ -574,6 +583,7 @@
     </font>
     <font>
       <name val="Calibri"/>
+      <family val="2"/>
       <b val="1"/>
       <sz val="11"/>
     </font>
@@ -732,8 +742,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="20" pivotButton="0" quotePrefix="1" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -755,6 +763,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="20" pivotButton="0" quotePrefix="1" xfId="0"/>
     <xf applyAlignment="1" borderId="5" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1031,7 +1043,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1046,7 +1058,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1066,111 +1078,111 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="23" t="n">
-        <v>192.759</v>
-      </c>
-      <c r="C2" s="29" t="n">
-        <v>-0.02300000000002456</v>
+      <c r="B2" s="21" t="n">
+        <v>181.685</v>
+      </c>
+      <c r="C2" s="27" t="n">
+        <v>0.2079999999999984</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="23" t="n">
-        <v>12095.12</v>
-      </c>
-      <c r="C3" s="29" t="n">
-        <v>-0.3913481746967595</v>
+      <c r="B3" s="21" t="n">
+        <v>12437.87</v>
+      </c>
+      <c r="C3" s="27" t="n">
+        <v>1.088184473641873</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="23" t="n">
-        <v>2.1674301</v>
-      </c>
-      <c r="C4" s="29" t="n">
-        <v>0.0004300999999999888</v>
+      <c r="B4" s="21" t="n">
+        <v>2.0913861</v>
+      </c>
+      <c r="C4" s="27" t="n">
+        <v>0.03938609999999976</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="23" t="n">
-        <v>2462.6</v>
-      </c>
-      <c r="C5" s="29" t="n">
-        <v>-0.4688384124161282</v>
+      <c r="B5" s="21" t="n">
+        <v>2474</v>
+      </c>
+      <c r="C5" s="27" t="n">
+        <v>0.5282405526208844</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="23" t="n">
-        <v>1.1909</v>
-      </c>
-      <c r="C6" s="29" t="n">
-        <v>0.4131534569983275</v>
+      <c r="B6" s="21" t="n">
+        <v>1.201</v>
+      </c>
+      <c r="C6" s="27" t="n">
+        <v>-0.2160186108341566</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="23" t="n">
-        <v>17.9194</v>
-      </c>
-      <c r="C7" s="29" t="n">
-        <v>0.5922341542278664</v>
-      </c>
-      <c r="H7" s="31" t="n"/>
+      <c r="B7" s="21" t="n">
+        <v>17.6809</v>
+      </c>
+      <c r="C7" s="27" t="n">
+        <v>-0.1722054721817634</v>
+      </c>
+      <c r="H7" s="29" t="n"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="23" t="n">
-        <v>47.3</v>
-      </c>
-      <c r="C8" s="29" t="n">
-        <v>0.02114611968704327</v>
+      <c r="B8" s="21" t="n">
+        <v>47.79</v>
+      </c>
+      <c r="C8" s="27" t="n">
+        <v>0.6529064869418733</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="23" t="n">
-        <v>582.5</v>
-      </c>
-      <c r="C9" s="29" t="n">
-        <v>0.8658008658008587</v>
+      <c r="B9" s="21" t="n">
+        <v>530</v>
+      </c>
+      <c r="C9" s="27" t="n">
+        <v>-2.84142988084326</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="23" t="n">
-        <v>949.5</v>
-      </c>
-      <c r="C10" s="29" t="n">
-        <v>0</v>
+      <c r="B10" s="21" t="n">
+        <v>963.75</v>
+      </c>
+      <c r="C10" s="27" t="n">
+        <v>0.1819126819126771</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="23" t="n">
-        <v>10.13</v>
-      </c>
-      <c r="C11" s="29" t="n">
-        <v>0</v>
+      <c r="B11" s="21" t="n">
+        <v>11.13</v>
+      </c>
+      <c r="C11" s="27" t="n">
+        <v>-0.9899999999999984</v>
       </c>
     </row>
   </sheetData>
@@ -1184,220 +1196,210 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="2" min="2" style="35" width="13.28515625"/>
-    <col customWidth="1" max="3" min="3" style="35" width="13.5703125"/>
-    <col customWidth="1" max="4" min="4" style="35" width="11.140625"/>
-    <col customWidth="1" max="5" min="5" style="35" width="15.28515625"/>
+    <col customWidth="1" max="2" min="2" style="33" width="13.28515625"/>
+    <col customWidth="1" max="3" min="3" style="33" width="13.5703125"/>
+    <col customWidth="1" max="4" min="4" style="33" width="11.140625"/>
+    <col customWidth="1" max="5" min="5" style="33" width="15.28515625"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15.75" r="1" s="35" spans="1:9" thickBot="1">
+    <row customHeight="1" ht="15.75" r="1" s="33" spans="1:5" thickBot="1">
       <c r="A1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="E1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="2" s="35" spans="1:9" thickBot="1">
+        <v>160</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="2" s="33" spans="1:5" thickBot="1">
       <c r="A2" s="14" t="s">
         <v>97</v>
       </c>
       <c r="B2" s="17" t="n">
-        <v>3201636</v>
+        <v>3283045</v>
       </c>
       <c r="C2" s="15" t="n">
-        <v>3325087</v>
+        <v>3174343</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>123451</v>
+        <v>-108702</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>37851402.656</v>
-      </c>
-      <c r="I2" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="3" s="35" spans="1:9" thickBot="1">
+        <v>26500470.208</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="3" s="33" spans="1:5" thickBot="1">
       <c r="A3" s="14" t="s">
         <v>98</v>
       </c>
       <c r="B3" s="17" t="n">
-        <v>271515</v>
+        <v>300720</v>
       </c>
       <c r="C3" s="15" t="n">
-        <v>284245</v>
+        <v>307775</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>12730</v>
+        <v>7055</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>2336378.467</v>
-      </c>
-      <c r="I3" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="4" s="35" spans="1:9" thickBot="1">
+        <v>717775.2929999999</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="4" s="33" spans="1:5" thickBot="1">
       <c r="A4" s="14" t="s">
         <v>99</v>
       </c>
       <c r="B4" s="17" t="n">
-        <v>263650</v>
+        <v>263655</v>
       </c>
       <c r="C4" s="15" t="n">
-        <v>261080</v>
+        <v>281130</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>-2570</v>
+        <v>17475</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>1261434.008</v>
-      </c>
-      <c r="I4" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="5" s="35" spans="1:9" thickBot="1">
+        <v>10054122.084</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="5" s="33" spans="1:5" thickBot="1">
       <c r="A5" s="14" t="s">
         <v>66</v>
       </c>
       <c r="B5" s="17" t="n">
-        <v>4157305</v>
+        <v>4213295</v>
       </c>
       <c r="C5" s="15" t="n">
-        <v>4116181</v>
+        <v>4221431</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>-41124</v>
+        <v>8136</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>41016202.002</v>
-      </c>
-      <c r="I5" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="6" s="35" spans="1:9" thickBot="1">
+        <v>24623767.295</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="6" s="33" spans="1:5" thickBot="1">
       <c r="A6" s="14" t="s">
         <v>100</v>
       </c>
       <c r="B6" s="17" t="n">
-        <v>72305</v>
+        <v>75650</v>
       </c>
       <c r="C6" s="15" t="n">
-        <v>73265</v>
+        <v>75655</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>960</v>
+        <v>5</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>196467.438</v>
-      </c>
-      <c r="I6" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="7" s="35" spans="1:9" thickBot="1">
+        <v>129265.17</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="7" s="33" spans="1:5" thickBot="1">
       <c r="A7" s="14" t="s">
         <v>101</v>
       </c>
       <c r="B7" s="17" t="n">
-        <v>52290</v>
+        <v>63750</v>
       </c>
       <c r="C7" s="15" t="n">
-        <v>56325</v>
+        <v>63765</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>4035</v>
+        <v>15</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>392451.178</v>
-      </c>
-      <c r="I7" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="8" s="35" spans="1:9" thickBot="1">
+        <v>118954.882</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="8" s="33" spans="1:5" thickBot="1">
       <c r="A8" s="14" t="s">
         <v>102</v>
       </c>
       <c r="B8" s="17" t="n">
-        <v>1205473</v>
+        <v>1245752</v>
       </c>
       <c r="C8" s="15" t="n">
-        <v>1241180</v>
+        <v>1276173</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>35707</v>
+        <v>30421</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>5587872.954</v>
-      </c>
-      <c r="I8" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="9" s="35" spans="1:9" thickBot="1">
+        <v>8122139.062</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="9" s="33" spans="1:5" thickBot="1">
       <c r="A9" s="14" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B9" s="17" t="n">
-        <v>25845</v>
+        <v>26330</v>
       </c>
       <c r="C9" s="15" t="n">
-        <v>25840</v>
+        <v>26330</v>
       </c>
       <c r="D9" s="3" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>477.12</v>
-      </c>
-      <c r="I9" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="10" s="35" spans="1:9" thickBot="1">
+        <v>2389.889</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="10" s="33" spans="1:5" thickBot="1">
       <c r="A10" s="14" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B10" s="17" t="n">
-        <v>35045</v>
+        <v>36370</v>
       </c>
       <c r="C10" s="15" t="n">
-        <v>35040</v>
+        <v>36370</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>236634.714</v>
-      </c>
-      <c r="I10" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="11" s="35" spans="1:9" thickBot="1">
+        <v>57982.836</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="11" s="33" spans="1:5" thickBot="1">
       <c r="A11" s="14" t="s">
         <v>103</v>
       </c>
       <c r="B11" s="17" t="n">
-        <v>1425844</v>
+        <v>1478483</v>
       </c>
       <c r="C11" s="15" t="n">
-        <v>1462190</v>
+        <v>1469898</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>36346</v>
+        <v>-8585</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>10303879.049</v>
-      </c>
-      <c r="I11" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="12" s="35" spans="1:9" thickBot="1">
+        <v>13739003.941</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="12" s="33" spans="1:5" thickBot="1">
       <c r="A12" s="14" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B12" s="17" t="n">
         <v>5485</v>
@@ -1411,17 +1413,16 @@
       <c r="E12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I12" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="13" s="35" spans="1:9" thickBot="1">
+    </row>
+    <row customHeight="1" ht="15.75" r="13" s="33" spans="1:5" thickBot="1">
       <c r="A13" s="14" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B13" s="17" t="n">
-        <v>0</v>
+        <v>4350</v>
       </c>
       <c r="C13" s="15" t="n">
-        <v>0</v>
+        <v>4350</v>
       </c>
       <c r="D13" s="3" t="n">
         <v>0</v>
@@ -1429,269 +1430,254 @@
       <c r="E13" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I13" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="14" s="35" spans="1:9" thickBot="1">
+    </row>
+    <row customHeight="1" ht="15.75" r="14" s="33" spans="1:5" thickBot="1">
       <c r="A14" s="14" t="s">
         <v>104</v>
       </c>
       <c r="B14" s="17" t="n">
-        <v>639145</v>
+        <v>635697</v>
       </c>
       <c r="C14" s="15" t="n">
-        <v>638172</v>
+        <v>641006</v>
       </c>
       <c r="D14" s="3" t="n">
-        <v>-973</v>
+        <v>5309</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>1105127.951</v>
-      </c>
-      <c r="I14" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="15" s="35" spans="1:9" thickBot="1">
+        <v>2887557.871</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="15" s="33" spans="1:5" thickBot="1">
       <c r="A15" s="14" t="s">
         <v>68</v>
       </c>
       <c r="B15" s="17" t="n">
-        <v>2324130</v>
+        <v>2322802</v>
       </c>
       <c r="C15" s="15" t="n">
-        <v>2311619</v>
+        <v>2122813</v>
       </c>
       <c r="D15" s="3" t="n">
-        <v>-12511</v>
+        <v>-199989</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>26319221.315</v>
-      </c>
-      <c r="I15" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="16" s="35" spans="1:9" thickBot="1">
+        <v>63759415.995</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="16" s="33" spans="1:5" thickBot="1">
       <c r="A16" s="14" t="s">
         <v>105</v>
       </c>
       <c r="B16" s="17" t="n">
-        <v>571054</v>
+        <v>567915</v>
       </c>
       <c r="C16" s="15" t="n">
-        <v>570588</v>
+        <v>568096</v>
       </c>
       <c r="D16" s="3" t="n">
-        <v>-466</v>
+        <v>181</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>376433.385</v>
-      </c>
-      <c r="I16" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="17" s="35" spans="1:9" thickBot="1">
+        <v>586644.303</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="17" s="33" spans="1:5" thickBot="1">
       <c r="A17" s="14" t="s">
         <v>106</v>
       </c>
       <c r="B17" s="17" t="n">
-        <v>541633</v>
+        <v>578021</v>
       </c>
       <c r="C17" s="15" t="n">
-        <v>560618</v>
+        <v>576951</v>
       </c>
       <c r="D17" s="3" t="n">
-        <v>18985</v>
+        <v>-1070</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>3636327.323</v>
-      </c>
-      <c r="I17" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="18" s="35" spans="1:9" thickBot="1">
+        <v>1406955.5</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="18" s="33" spans="1:5" thickBot="1">
       <c r="A18" s="14" t="s">
         <v>107</v>
       </c>
       <c r="B18" s="17" t="n">
-        <v>245172</v>
+        <v>260090</v>
       </c>
       <c r="C18" s="15" t="n">
-        <v>247960</v>
+        <v>266755</v>
       </c>
       <c r="D18" s="3" t="n">
-        <v>2788</v>
+        <v>6665</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>1014757.968</v>
-      </c>
-      <c r="I18" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="19" s="35" spans="1:9" thickBot="1">
+        <v>1614306.312</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="19" s="33" spans="1:5" thickBot="1">
       <c r="A19" s="14" t="s">
         <v>108</v>
       </c>
       <c r="B19" s="17" t="n">
-        <v>1740801</v>
+        <v>1640716</v>
       </c>
       <c r="C19" s="15" t="n">
-        <v>1733381</v>
+        <v>1724560</v>
       </c>
       <c r="D19" s="3" t="n">
-        <v>-7420</v>
+        <v>83844</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>11549187.927</v>
-      </c>
-      <c r="I19" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="20" s="35" spans="1:9" thickBot="1">
+        <v>18120066.744</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="20" s="33" spans="1:5" thickBot="1">
       <c r="A20" s="14" t="s">
         <v>109</v>
       </c>
       <c r="B20" s="17" t="n">
-        <v>74724</v>
+        <v>73894</v>
       </c>
       <c r="C20" s="15" t="n">
-        <v>74009</v>
+        <v>74059</v>
       </c>
       <c r="D20" s="3" t="n">
-        <v>-715</v>
+        <v>165</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>92080.808</v>
-      </c>
-      <c r="I20" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="21" s="35" spans="1:9" thickBot="1">
+        <v>45518.782</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="21" s="33" spans="1:5" thickBot="1">
       <c r="A21" s="14" t="s">
         <v>110</v>
       </c>
       <c r="B21" s="17" t="n">
-        <v>1322484</v>
+        <v>1320914</v>
       </c>
       <c r="C21" s="15" t="n">
-        <v>1319534</v>
+        <v>1322156</v>
       </c>
       <c r="D21" s="3" t="n">
-        <v>-2950</v>
+        <v>1242</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>3483983.058</v>
-      </c>
-      <c r="I21" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="22" s="35" spans="1:9" thickBot="1">
+        <v>1514029.217</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="22" s="33" spans="1:5" thickBot="1">
       <c r="A22" s="14" t="s">
         <v>111</v>
       </c>
       <c r="B22" s="17" t="n">
-        <v>50090</v>
+        <v>49642</v>
       </c>
       <c r="C22" s="15" t="n">
-        <v>50070</v>
+        <v>50182</v>
       </c>
       <c r="D22" s="3" t="n">
-        <v>-20</v>
+        <v>540</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>116804.731</v>
-      </c>
-      <c r="I22" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="23" s="35" spans="1:9" thickBot="1">
+        <v>46434.494</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="23" s="33" spans="1:5" thickBot="1">
       <c r="A23" s="14" t="s">
         <v>69</v>
       </c>
       <c r="B23" s="17" t="n">
-        <v>1430247</v>
+        <v>1459181</v>
       </c>
       <c r="C23" s="15" t="n">
-        <v>1443515</v>
+        <v>1462307</v>
       </c>
       <c r="D23" s="3" t="n">
-        <v>13268</v>
+        <v>3126</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>12790765.561</v>
-      </c>
-      <c r="I23" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="24" s="35" spans="1:9" thickBot="1">
+        <v>12443911.026</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="24" s="33" spans="1:5" thickBot="1">
       <c r="A24" s="14" t="s">
         <v>112</v>
       </c>
       <c r="B24" s="17" t="n">
-        <v>33750</v>
+        <v>33895</v>
       </c>
       <c r="C24" s="15" t="n">
-        <v>33580</v>
+        <v>33865</v>
       </c>
       <c r="D24" s="3" t="n">
-        <v>-170</v>
+        <v>-30</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>41155.105</v>
-      </c>
-      <c r="I24" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="25" s="35" spans="1:9" thickBot="1">
+        <v>8843.678</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="25" s="33" spans="1:5" thickBot="1">
       <c r="A25" s="14" t="s">
         <v>113</v>
       </c>
       <c r="B25" s="17" t="n">
-        <v>219196</v>
+        <v>247984</v>
       </c>
       <c r="C25" s="15" t="n">
-        <v>228438</v>
+        <v>259768</v>
       </c>
       <c r="D25" s="3" t="n">
-        <v>9242</v>
+        <v>11784</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>1628640.824</v>
-      </c>
-      <c r="I25" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="26" s="35" spans="1:9" thickBot="1">
+        <v>2165597.257</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="26" s="33" spans="1:5" thickBot="1">
       <c r="A26" s="14" t="s">
         <v>114</v>
       </c>
       <c r="B26" s="17" t="n">
-        <v>17062</v>
+        <v>17057</v>
       </c>
       <c r="C26" s="15" t="n">
-        <v>17062</v>
+        <v>17092</v>
       </c>
       <c r="D26" s="3" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>3115.788</v>
-      </c>
-      <c r="I26" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="27" s="35" spans="1:9" thickBot="1">
+        <v>12249.958</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="27" s="33" spans="1:5" thickBot="1">
       <c r="A27" s="14" t="s">
         <v>115</v>
       </c>
       <c r="B27" s="17" t="n">
-        <v>106219</v>
+        <v>109549</v>
       </c>
       <c r="C27" s="15" t="n">
-        <v>106649</v>
+        <v>111379</v>
       </c>
       <c r="D27" s="3" t="n">
-        <v>430</v>
+        <v>1830</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>296828.47</v>
-      </c>
-      <c r="I27" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="28" s="35" spans="1:9" thickBot="1">
+        <v>865518.6580000001</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="28" s="33" spans="1:5" thickBot="1">
       <c r="A28" s="14" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B28" s="17" t="n">
-        <v>1805</v>
+        <v>1590</v>
       </c>
       <c r="C28" s="15" t="n">
-        <v>1805</v>
+        <v>1590</v>
       </c>
       <c r="D28" s="3" t="n">
         <v>0</v>
@@ -1699,45 +1685,42 @@
       <c r="E28" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I28" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="29" s="35" spans="1:9" thickBot="1">
+    </row>
+    <row customHeight="1" ht="15.75" r="29" s="33" spans="1:5" thickBot="1">
       <c r="A29" s="14" t="s">
         <v>116</v>
       </c>
       <c r="B29" s="17" t="n">
-        <v>12815</v>
+        <v>11995</v>
       </c>
       <c r="C29" s="15" t="n">
-        <v>12815</v>
+        <v>12000</v>
       </c>
       <c r="D29" s="3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>11554.762</v>
-      </c>
-      <c r="I29" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="30" s="35" spans="1:9" thickBot="1">
+        <v>324.843</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="30" s="33" spans="1:5" thickBot="1">
       <c r="A30" s="14" t="s">
         <v>70</v>
       </c>
       <c r="B30" s="17" t="n">
-        <v>766254</v>
+        <v>761521</v>
       </c>
       <c r="C30" s="15" t="n">
-        <v>761147</v>
+        <v>762546</v>
       </c>
       <c r="D30" s="3" t="n">
-        <v>-5107</v>
+        <v>1025</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>3179710.749</v>
-      </c>
-      <c r="I30" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="31" s="35" spans="1:9" thickBot="1">
+        <v>3941801.081</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="31" s="33" spans="1:5" thickBot="1">
       <c r="A31" s="14" t="s">
         <v>117</v>
       </c>
@@ -1753,27 +1736,25 @@
       <c r="E31" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I31" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="32" s="35" spans="1:9" thickBot="1">
+    </row>
+    <row customHeight="1" ht="15.75" r="32" s="33" spans="1:5" thickBot="1">
       <c r="A32" s="14" t="s">
         <v>118</v>
       </c>
       <c r="B32" s="17" t="n">
-        <v>57145</v>
+        <v>57015</v>
       </c>
       <c r="C32" s="15" t="n">
-        <v>57145</v>
+        <v>56990</v>
       </c>
       <c r="D32" s="3" t="n">
-        <v>0</v>
+        <v>-25</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>2478.522</v>
-      </c>
-      <c r="I32" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="33" s="35" spans="1:9" thickBot="1">
+        <v>26613.342</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="33" s="33" spans="1:5" thickBot="1">
       <c r="A33" s="14" t="s">
         <v>119</v>
       </c>
@@ -1789,63 +1770,59 @@
       <c r="E33" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I33" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="34" s="35" spans="1:9" thickBot="1">
+    </row>
+    <row customHeight="1" ht="15.75" r="34" s="33" spans="1:5" thickBot="1">
       <c r="A34" s="14" t="s">
         <v>71</v>
       </c>
       <c r="B34" s="17" t="n">
-        <v>545352</v>
+        <v>525545</v>
       </c>
       <c r="C34" s="15" t="n">
-        <v>544316</v>
+        <v>524796</v>
       </c>
       <c r="D34" s="3" t="n">
-        <v>-1036</v>
+        <v>-749</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>2115929.942</v>
-      </c>
-      <c r="I34" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="35" s="35" spans="1:9" thickBot="1">
+        <v>2091885.214</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="35" s="33" spans="1:5" thickBot="1">
       <c r="A35" s="14" t="s">
         <v>120</v>
       </c>
       <c r="B35" s="17" t="n">
-        <v>61868</v>
+        <v>62683</v>
       </c>
       <c r="C35" s="15" t="n">
-        <v>62018</v>
+        <v>62683</v>
       </c>
       <c r="D35" s="3" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>85824.022</v>
-      </c>
-      <c r="I35" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="36" s="35" spans="1:9" thickBot="1">
+        <v>66722.49800000001</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="36" s="33" spans="1:5" thickBot="1">
       <c r="A36" s="14" t="s">
         <v>72</v>
       </c>
       <c r="B36" s="18" t="n">
-        <v>397268</v>
+        <v>412545</v>
       </c>
       <c r="C36" s="16" t="n">
-        <v>406443</v>
+        <v>414113</v>
       </c>
       <c r="D36" s="3" t="n">
-        <v>9175</v>
+        <v>1568</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>1781981.08</v>
-      </c>
-      <c r="I36" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="37" s="35" spans="1:9" thickBot="1">
+        <v>996471.106</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="37" s="33" spans="1:5" thickBot="1">
       <c r="A37" s="14" t="s">
         <v>121</v>
       </c>
@@ -1861,17 +1838,16 @@
       <c r="E37" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I37" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="38" s="35" spans="1:9" thickBot="1">
+    </row>
+    <row customHeight="1" ht="15.75" r="38" s="33" spans="1:5" thickBot="1">
       <c r="A38" s="14" t="s">
         <v>122</v>
       </c>
       <c r="B38" s="18" t="n">
-        <v>4487</v>
+        <v>4562</v>
       </c>
       <c r="C38" s="16" t="n">
-        <v>4487</v>
+        <v>4562</v>
       </c>
       <c r="D38" s="3" t="n">
         <v>0</v>
@@ -1879,9 +1855,8 @@
       <c r="E38" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I38" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="39" s="35" spans="1:9" thickBot="1">
+    </row>
+    <row customHeight="1" ht="15.75" r="39" s="33" spans="1:5" thickBot="1">
       <c r="A39" s="1" t="s">
         <v>123</v>
       </c>
@@ -1891,11 +1866,14 @@
       <c r="C39" s="5" t="n">
         <v>1215</v>
       </c>
-      <c r="D39" s="3" t="n"/>
-      <c r="E39" s="6" t="n"/>
-      <c r="I39" s="21" t="n"/>
-    </row>
-    <row customHeight="1" ht="15.75" r="40" s="35" spans="1:9" thickBot="1">
+      <c r="D39" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="40" s="33" spans="1:5" thickBot="1">
       <c r="A40" s="1" t="n"/>
       <c r="B40" s="7" t="n"/>
       <c r="C40" s="6" t="n"/>
@@ -1917,17 +1895,17 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1945,13 +1923,13 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="35" width="20.140625"/>
-    <col bestFit="1" customWidth="1" max="11" min="11" style="35" width="9.7109375"/>
+    <col customWidth="1" max="1" min="1" style="33" width="20.140625"/>
+    <col bestFit="1" customWidth="1" max="11" min="11" style="33" width="9.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -2165,15 +2143,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F190"/>
+  <dimension ref="A1:F204"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="A193" sqref="A193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="35" width="10.7109375"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="33" width="10.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2186,7 +2164,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="11">
-        <f>_xll.BDH(E3,B1,$F4,"","cols=2;rows=189")</f>
+        <f>_xll.BDH(E3,B1,$F4,"","cols=2;rows=191")</f>
         <v/>
       </c>
       <c r="B2" t="n">
@@ -3705,6 +3683,58 @@
       <c r="B190" t="n">
         <v>9.210000000000001</v>
       </c>
+    </row>
+    <row r="191" spans="1:6">
+      <c r="A191" s="20" t="n">
+        <v>42982</v>
+      </c>
+      <c r="B191" t="n">
+        <v>9.199999999999999</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6">
+      <c r="A192" s="20" t="n">
+        <v>42983</v>
+      </c>
+      <c r="B192" t="n">
+        <v>9.07</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6">
+      <c r="A193" s="20" t="n"/>
+    </row>
+    <row r="194" spans="1:6">
+      <c r="A194" s="20" t="n"/>
+    </row>
+    <row r="195" spans="1:6">
+      <c r="A195" s="20" t="n"/>
+    </row>
+    <row r="196" spans="1:6">
+      <c r="A196" s="20" t="n"/>
+    </row>
+    <row r="197" spans="1:6">
+      <c r="A197" s="20" t="n"/>
+    </row>
+    <row r="198" spans="1:6">
+      <c r="A198" s="20" t="n"/>
+    </row>
+    <row r="199" spans="1:6">
+      <c r="A199" s="20" t="n"/>
+    </row>
+    <row r="200" spans="1:6">
+      <c r="A200" s="20" t="n"/>
+    </row>
+    <row r="201" spans="1:6">
+      <c r="A201" s="20" t="n"/>
+    </row>
+    <row r="202" spans="1:6">
+      <c r="A202" s="20" t="n"/>
+    </row>
+    <row r="203" spans="1:6">
+      <c r="A203" s="20" t="n"/>
+    </row>
+    <row r="204" spans="1:6">
+      <c r="A204" s="20" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -3720,13 +3750,13 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A15"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="35" width="9.140625"/>
-    <col customWidth="1" max="9" min="9" style="35" width="9.140625"/>
+    <col customWidth="1" max="1" min="1" style="33" width="9.140625"/>
+    <col customWidth="1" max="9" min="9" style="33" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -3768,40 +3798,40 @@
       <c r="A2" s="9" t="n">
         <v>43327</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="25" t="s">
         <v>44</v>
       </c>
       <c r="C2" s="10" t="n">
-        <v>3.39</v>
-      </c>
-      <c r="D2" s="23" t="n">
-        <v>0.03999999999999976</v>
-      </c>
-      <c r="E2" s="23" t="n">
-        <v>4.046559801487604</v>
-      </c>
-      <c r="F2" s="23" t="n">
-        <v>-0.009502435846675539</v>
-      </c>
-      <c r="G2" s="23" t="n">
+        <v>3.37</v>
+      </c>
+      <c r="D2" s="21" t="n">
+        <v>-0.009999999999999593</v>
+      </c>
+      <c r="E2" s="21" t="n">
+        <v>3.892371823943463</v>
+      </c>
+      <c r="F2" s="21" t="n">
+        <v>-0.03345670489529606</v>
+      </c>
+      <c r="G2" s="21" t="n">
         <v>0</v>
       </c>
-      <c r="H2" s="23" t="n">
+      <c r="H2" s="21" t="n">
         <v>0</v>
       </c>
-      <c r="I2" s="28" t="n">
-        <v>43986</v>
-      </c>
-      <c r="J2" s="26" t="n">
-        <v>8319.515493093595</v>
+      <c r="I2" s="26" t="n">
+        <v>43987</v>
+      </c>
+      <c r="J2" s="24" t="n">
+        <v>8323.396506376706</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.03876928074922348</v>
+        <v>0.08144721886760298</v>
       </c>
       <c r="L2" t="n">
-        <v>0.08886811367086758</v>
-      </c>
-      <c r="P2" s="27" t="s">
+        <v>0.08603240388500437</v>
+      </c>
+      <c r="P2" s="25" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3809,40 +3839,40 @@
       <c r="A3" s="9" t="n">
         <v>43600</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="25" t="s">
         <v>46</v>
       </c>
       <c r="C3" s="10" t="n">
-        <v>3.39</v>
-      </c>
-      <c r="D3" s="23" t="n">
-        <v>0.01270000000000021</v>
-      </c>
-      <c r="E3" s="23" t="n">
-        <v>4.502935036586564</v>
-      </c>
-      <c r="F3" s="23" t="n">
-        <v>0.01777198053978246</v>
-      </c>
-      <c r="G3" s="23" t="n">
-        <v>3.39</v>
-      </c>
-      <c r="H3" s="23" t="n">
-        <v>3.39</v>
-      </c>
-      <c r="I3" s="28" t="n">
+        <v>3.338</v>
+      </c>
+      <c r="D3" s="21" t="n">
+        <v>-0.004599999999999743</v>
+      </c>
+      <c r="E3" s="21" t="n">
+        <v>4.342828889848627</v>
+      </c>
+      <c r="F3" s="21" t="n">
+        <v>-0.01342946074334161</v>
+      </c>
+      <c r="G3" s="21" t="n">
+        <v>3.338</v>
+      </c>
+      <c r="H3" s="21" t="n">
+        <v>3.338</v>
+      </c>
+      <c r="I3" s="26" t="n">
         <v>44196</v>
       </c>
-      <c r="J3" s="26" t="n">
-        <v>10244.83004307429</v>
+      <c r="J3" s="24" t="n">
+        <v>10271.99435065842</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.008505095244470962</v>
+        <v>0.0903733689978925</v>
       </c>
       <c r="L3" t="n">
-        <v>0.09208305731622317</v>
-      </c>
-      <c r="P3" s="27">
+        <v>0.08909410674705413</v>
+      </c>
+      <c r="P3" s="25">
         <f>"B"&amp;TEXT(O3,"A")</f>
         <v/>
       </c>
@@ -3851,40 +3881,40 @@
       <c r="A4" s="9" t="n">
         <v>44058</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="25" t="s">
         <v>47</v>
       </c>
       <c r="C4" s="10" t="n">
-        <v>4.1141</v>
-      </c>
-      <c r="D4" s="23" t="n">
-        <v>0.01410000000000022</v>
-      </c>
-      <c r="E4" s="23" t="n">
-        <v>4.661902904855619</v>
-      </c>
-      <c r="F4" s="23" t="n">
-        <v>0.01659294007043677</v>
-      </c>
-      <c r="G4" s="23" t="n">
-        <v>4.1141</v>
-      </c>
-      <c r="H4" s="23" t="n">
-        <v>4.661902904855619</v>
-      </c>
-      <c r="I4" s="28" t="n">
+        <v>3.98</v>
+      </c>
+      <c r="D4" s="21" t="n">
+        <v>-0.05000000000000004</v>
+      </c>
+      <c r="E4" s="21" t="n">
+        <v>4.528655032667706</v>
+      </c>
+      <c r="F4" s="21" t="n">
+        <v>0.01379710722320127</v>
+      </c>
+      <c r="G4" s="21" t="n">
+        <v>3.98</v>
+      </c>
+      <c r="H4" s="21" t="n">
+        <v>4.528655032667706</v>
+      </c>
+      <c r="I4" s="26" t="n">
         <v>44578</v>
       </c>
-      <c r="J4" s="26" t="n">
-        <v>13279.5223959777</v>
+      <c r="J4" s="24" t="n">
+        <v>13351.02789607177</v>
       </c>
       <c r="K4" t="n">
-        <v>0.02189101647086245</v>
+        <v>0.09733769124220526</v>
       </c>
       <c r="L4" t="n">
-        <v>0.09618328207909679</v>
-      </c>
-      <c r="P4" s="27">
+        <v>0.09331856594920095</v>
+      </c>
+      <c r="P4" s="25">
         <f>"B"&amp;TEXT(O4,"A")</f>
         <v/>
       </c>
@@ -3893,40 +3923,40 @@
       <c r="A5" s="9" t="n">
         <v>44331</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="25" t="s">
         <v>48</v>
       </c>
       <c r="C5" s="10" t="n">
-        <v>4.31</v>
-      </c>
-      <c r="D5" s="23" t="n">
-        <v>0.01570000000000044</v>
-      </c>
-      <c r="E5" s="23" t="n">
-        <v>4.794395785707772</v>
-      </c>
-      <c r="F5" s="23" t="n">
-        <v>0.005866541177335094</v>
-      </c>
-      <c r="G5" s="23" t="n">
-        <v>5.244547274305034</v>
-      </c>
-      <c r="H5" s="23" t="n">
-        <v>5.425341212262458</v>
-      </c>
-      <c r="I5" s="28" t="n">
-        <v>44756</v>
-      </c>
-      <c r="J5" s="26" t="n">
-        <v>14991.53230755394</v>
+        <v>4.17</v>
+      </c>
+      <c r="D5" s="21" t="n">
+        <v>-0.03429999999999961</v>
+      </c>
+      <c r="E5" s="21" t="n">
+        <v>4.655807466897155</v>
+      </c>
+      <c r="F5" s="21" t="n">
+        <v>-0.006835896871226765</v>
+      </c>
+      <c r="G5" s="21" t="n">
+        <v>5.078584208844261</v>
+      </c>
+      <c r="H5" s="21" t="n">
+        <v>5.262785655024826</v>
+      </c>
+      <c r="I5" s="26" t="n">
+        <v>44757</v>
+      </c>
+      <c r="J5" s="24" t="n">
+        <v>15100.54080963903</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0295670883986715</v>
+        <v>0.09655323054025278</v>
       </c>
       <c r="L5" t="n">
-        <v>0.09755837506371245</v>
-      </c>
-      <c r="P5" s="27">
+        <v>0.09434924802024647</v>
+      </c>
+      <c r="P5" s="25">
         <f>"B"&amp;TEXT(O5,"A")</f>
         <v/>
       </c>
@@ -3935,40 +3965,40 @@
       <c r="A6" s="9" t="n">
         <v>44788</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="25" t="s">
         <v>49</v>
       </c>
       <c r="C6" s="10" t="n">
-        <v>4.62</v>
-      </c>
-      <c r="D6" s="23" t="n">
-        <v>0.006799999999999862</v>
-      </c>
-      <c r="E6" s="23" t="n">
-        <v>4.836284186183515</v>
-      </c>
-      <c r="F6" s="23" t="n">
-        <v>0.01299332965614131</v>
-      </c>
-      <c r="G6" s="23" t="n">
-        <v>5.611744936412322</v>
-      </c>
-      <c r="H6" s="23" t="n">
-        <v>4.969574995157822</v>
-      </c>
-      <c r="I6" s="28" t="n">
-        <v>45111</v>
-      </c>
-      <c r="J6" s="26" t="n">
-        <v>17881.37100336955</v>
+        <v>4.48</v>
+      </c>
+      <c r="D6" s="21" t="n">
+        <v>-0.02999999999999947</v>
+      </c>
+      <c r="E6" s="21" t="n">
+        <v>4.672853014499623</v>
+      </c>
+      <c r="F6" s="21" t="n">
+        <v>-0.01207127862508095</v>
+      </c>
+      <c r="G6" s="21" t="n">
+        <v>5.466968455193966</v>
+      </c>
+      <c r="H6" s="21" t="n">
+        <v>4.726805500807174</v>
+      </c>
+      <c r="I6" s="26" t="n">
+        <v>45112</v>
+      </c>
+      <c r="J6" s="24" t="n">
+        <v>18051.25959605138</v>
       </c>
       <c r="K6" t="n">
-        <v>0.02701063662742531</v>
+        <v>0.08276837529901104</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0992335344475643</v>
-      </c>
-      <c r="P6" s="27">
+        <v>0.09591328945458021</v>
+      </c>
+      <c r="P6" s="25">
         <f>"B"&amp;TEXT(O6,"A")</f>
         <v/>
       </c>
@@ -3977,40 +4007,40 @@
       <c r="A7" s="9" t="n">
         <v>45061</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="25" t="s">
         <v>50</v>
       </c>
       <c r="C7" s="10" t="n">
-        <v>4.74</v>
-      </c>
-      <c r="D7" s="23" t="n">
-        <v>0.01650000000000054</v>
-      </c>
-      <c r="E7" s="23" t="n">
-        <v>4.825514619680371</v>
-      </c>
-      <c r="F7" s="23" t="n">
-        <v>0.004236206621532901</v>
-      </c>
-      <c r="G7" s="23" t="n">
-        <v>5.814377979541074</v>
-      </c>
-      <c r="H7" s="23" t="n">
-        <v>4.729687962125029</v>
-      </c>
-      <c r="I7" s="28" t="n">
-        <v>45587</v>
-      </c>
-      <c r="J7" s="26" t="n">
-        <v>21891.44288274428</v>
+        <v>4.59</v>
+      </c>
+      <c r="D7" s="21" t="n">
+        <v>-0.0446000000000002</v>
+      </c>
+      <c r="E7" s="21" t="n">
+        <v>4.66994399607068</v>
+      </c>
+      <c r="F7" s="21" t="n">
+        <v>-0.004259992708388616</v>
+      </c>
+      <c r="G7" s="21" t="n">
+        <v>5.562828328226255</v>
+      </c>
+      <c r="H7" s="21" t="n">
+        <v>4.644352810479191</v>
+      </c>
+      <c r="I7" s="26" t="n">
+        <v>45590</v>
+      </c>
+      <c r="J7" s="24" t="n">
+        <v>22198.90764833882</v>
       </c>
       <c r="K7" t="n">
-        <v>0.03349477169532766</v>
+        <v>0.07801190041768769</v>
       </c>
       <c r="L7" t="n">
-        <v>0.1014165688824119</v>
-      </c>
-      <c r="P7" s="27">
+        <v>0.09794188732373797</v>
+      </c>
+      <c r="P7" s="25">
         <f>"B"&amp;TEXT(O7,"A")</f>
         <v/>
       </c>
@@ -4019,40 +4049,40 @@
       <c r="A8" s="9" t="n">
         <v>45519</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="25" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="10" t="n">
-        <v>4.7744</v>
-      </c>
-      <c r="D8" s="23" t="n">
-        <v>0.01600000000000004</v>
-      </c>
-      <c r="E8" s="23" t="n">
-        <v>4.980152405321503</v>
-      </c>
-      <c r="F8" s="23" t="n">
-        <v>0.01004468913927692</v>
-      </c>
-      <c r="G8" s="23" t="n">
-        <v>4.946995005241139</v>
-      </c>
-      <c r="H8" s="23" t="n">
-        <v>5.758694545294074</v>
-      </c>
-      <c r="I8" s="28" t="n">
-        <v>46400</v>
-      </c>
-      <c r="J8" s="26" t="n">
-        <v>29010.44291846453</v>
+        <v>4.6234</v>
+      </c>
+      <c r="D8" s="21" t="n">
+        <v>-0.04399999999999959</v>
+      </c>
+      <c r="E8" s="21" t="n">
+        <v>4.807690328936931</v>
+      </c>
+      <c r="F8" s="21" t="n">
+        <v>-0.01530594300578336</v>
+      </c>
+      <c r="G8" s="21" t="n">
+        <v>4.790560058577475</v>
+      </c>
+      <c r="H8" s="21" t="n">
+        <v>5.499145895327362</v>
+      </c>
+      <c r="I8" s="26" t="n">
+        <v>46412</v>
+      </c>
+      <c r="J8" s="24" t="n">
+        <v>29606.72054304952</v>
       </c>
       <c r="K8" t="n">
-        <v>0.03093778284730953</v>
+        <v>0.06447780266274905</v>
       </c>
       <c r="L8" t="n">
-        <v>0.1036272801190787</v>
-      </c>
-      <c r="P8" s="27">
+        <v>0.100253972246511</v>
+      </c>
+      <c r="P8" s="25">
         <f>"B"&amp;TEXT(O8,"A")</f>
         <v/>
       </c>
@@ -4061,40 +4091,40 @@
       <c r="A9" s="9" t="n">
         <v>46249</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="25" t="s">
         <v>52</v>
       </c>
       <c r="C9" s="10" t="n">
-        <v>4.9783</v>
-      </c>
-      <c r="D9" s="23" t="n">
-        <v>0.03829999999999945</v>
-      </c>
-      <c r="E9" s="23" t="n">
-        <v>4.962696439380987</v>
-      </c>
-      <c r="F9" s="23" t="n">
-        <v>-0.01203876803934634</v>
-      </c>
-      <c r="G9" s="23" t="n">
-        <v>5.888569041791425</v>
-      </c>
-      <c r="H9" s="23" t="n">
-        <v>4.885214274129557</v>
-      </c>
-      <c r="I9" s="28" t="n">
-        <v>47126</v>
-      </c>
-      <c r="J9" s="26" t="n">
-        <v>36087.1642688127</v>
+        <v>4.81</v>
+      </c>
+      <c r="D9" s="21" t="n">
+        <v>-0.05740000000000051</v>
+      </c>
+      <c r="E9" s="21" t="n">
+        <v>4.813335925408646</v>
+      </c>
+      <c r="F9" s="21" t="n">
+        <v>-0.01664693749199309</v>
+      </c>
+      <c r="G9" s="21" t="n">
+        <v>5.63591167387778</v>
+      </c>
+      <c r="H9" s="21" t="n">
+        <v>4.838207459996369</v>
+      </c>
+      <c r="I9" s="26" t="n">
+        <v>47149</v>
+      </c>
+      <c r="J9" s="24" t="n">
+        <v>37089.47488243038</v>
       </c>
       <c r="K9" t="n">
-        <v>0.0269385213473583</v>
+        <v>0.05423725913035471</v>
       </c>
       <c r="L9" t="n">
-        <v>0.1041294807299652</v>
-      </c>
-      <c r="P9" s="27">
+        <v>0.1007439094663722</v>
+      </c>
+      <c r="P9" s="25">
         <f>"B"&amp;TEXT(O9,"A")</f>
         <v/>
       </c>
@@ -4103,40 +4133,40 @@
       <c r="A10" s="9" t="n">
         <v>47710</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C10" s="10" t="n">
-        <v>5.1047</v>
-      </c>
-      <c r="D10" s="23" t="n">
-        <v>0.004700000000000537</v>
-      </c>
-      <c r="E10" s="23" t="n">
-        <v>4.969363939541838</v>
-      </c>
-      <c r="F10" s="23" t="n">
-        <v>0.02688485286064246</v>
-      </c>
-      <c r="G10" s="23" t="n">
-        <v>5.510476192999003</v>
-      </c>
-      <c r="H10" s="23" t="n">
-        <v>4.99071710278074</v>
-      </c>
-      <c r="I10" s="28" t="n">
-        <v>47847</v>
-      </c>
-      <c r="J10" s="26" t="n">
-        <v>42133.28938402139</v>
+        <v>4.93</v>
+      </c>
+      <c r="D10" s="21" t="n">
+        <v>-0.05740000000000051</v>
+      </c>
+      <c r="E10" s="21" t="n">
+        <v>4.85932659008359</v>
+      </c>
+      <c r="F10" s="21" t="n">
+        <v>-0.02216108279169404</v>
+      </c>
+      <c r="G10" s="21" t="n">
+        <v>5.311548135310895</v>
+      </c>
+      <c r="H10" s="21" t="n">
+        <v>5.005341894830639</v>
+      </c>
+      <c r="I10" s="26" t="n">
+        <v>47889</v>
+      </c>
+      <c r="J10" s="24" t="n">
+        <v>43571.49118614896</v>
       </c>
       <c r="K10" t="n">
-        <v>0.02446389747001732</v>
+        <v>0.04756039259048994</v>
       </c>
       <c r="L10" t="n">
-        <v>0.1046042130817313</v>
-      </c>
-      <c r="P10" s="27">
+        <v>0.101743909466372</v>
+      </c>
+      <c r="P10" s="25">
         <f>"B"&amp;TEXT(O10,"A")</f>
         <v/>
       </c>
@@ -4145,40 +4175,40 @@
       <c r="A11" s="9" t="n">
         <v>49444</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="25" t="s">
         <v>54</v>
       </c>
       <c r="C11" s="10" t="n">
-        <v>5.1444</v>
-      </c>
-      <c r="D11" s="23" t="n">
-        <v>-0.002999999999999531</v>
-      </c>
-      <c r="E11" s="23" t="n">
-        <v>4.962090538578079</v>
-      </c>
-      <c r="F11" s="23" t="n">
-        <v>0.04496934460194169</v>
-      </c>
-      <c r="G11" s="23" t="n">
-        <v>5.332239438022945</v>
-      </c>
-      <c r="H11" s="23" t="n">
-        <v>4.927720660127077</v>
-      </c>
-      <c r="I11" s="28" t="n">
-        <v>48218</v>
-      </c>
-      <c r="J11" s="26" t="n">
-        <v>45657.40002395361</v>
+        <v>4.9631</v>
+      </c>
+      <c r="D11" s="21" t="n">
+        <v>-0.05219999999999947</v>
+      </c>
+      <c r="E11" s="21" t="n">
+        <v>4.950960661336268</v>
+      </c>
+      <c r="F11" s="21" t="n">
+        <v>-0.02829710846694589</v>
+      </c>
+      <c r="G11" s="21" t="n">
+        <v>5.11715876486547</v>
+      </c>
+      <c r="H11" s="21" t="n">
+        <v>5.378130312192431</v>
+      </c>
+      <c r="I11" s="26" t="n">
+        <v>48277</v>
+      </c>
+      <c r="J11" s="24" t="n">
+        <v>47410.61259050768</v>
       </c>
       <c r="K11" t="n">
-        <v>0.02582271683648774</v>
+        <v>0.04722560457422198</v>
       </c>
       <c r="L11" t="n">
-        <v>0.1046042130817313</v>
-      </c>
-      <c r="P11" s="27">
+        <v>0.102143909466372</v>
+      </c>
+      <c r="P11" s="25">
         <f>"B"&amp;TEXT(O11,"A")</f>
         <v/>
       </c>
@@ -4187,40 +4217,40 @@
       <c r="A12" s="9" t="n">
         <v>51363</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="25" t="s">
         <v>55</v>
       </c>
       <c r="C12" s="10" t="n">
-        <v>5.1952</v>
-      </c>
-      <c r="D12" s="23" t="n">
-        <v>0.002499999999999725</v>
-      </c>
-      <c r="E12" s="23" t="n">
-        <v>4.931494106746537</v>
-      </c>
-      <c r="F12" s="23" t="n">
-        <v>0.04511744082911218</v>
-      </c>
-      <c r="G12" s="23" t="n">
-        <v>5.48657203669396</v>
-      </c>
-      <c r="H12" s="23" t="n">
-        <v>4.756459667293478</v>
-      </c>
-      <c r="I12" s="28" t="n">
-        <v>48703</v>
-      </c>
-      <c r="J12" s="26" t="n">
-        <v>49679.9016828579</v>
+        <v>5.0136</v>
+      </c>
+      <c r="D12" s="21" t="n">
+        <v>-0.0564000000000002</v>
+      </c>
+      <c r="E12" s="21" t="n">
+        <v>4.972019115831872</v>
+      </c>
+      <c r="F12" s="21" t="n">
+        <v>-0.02442455370392782</v>
+      </c>
+      <c r="G12" s="21" t="n">
+        <v>5.297705085495052</v>
+      </c>
+      <c r="H12" s="21" t="n">
+        <v>5.090380807515893</v>
+      </c>
+      <c r="I12" s="26" t="n">
+        <v>48780</v>
+      </c>
+      <c r="J12" s="24" t="n">
+        <v>51885.64678713486</v>
       </c>
       <c r="K12" t="n">
-        <v>0.0232238810665697</v>
+        <v>0.04258963257369741</v>
       </c>
       <c r="L12" t="n">
-        <v>0.104604274412418</v>
-      </c>
-      <c r="P12" s="27">
+        <v>0.102106449606817</v>
+      </c>
+      <c r="P12" s="25">
         <f>"B"&amp;TEXT(O12,"A")</f>
         <v/>
       </c>
@@ -4229,40 +4259,40 @@
       <c r="A13" s="9" t="n">
         <v>53097</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="25" t="s">
         <v>56</v>
       </c>
       <c r="C13" s="10" t="n">
-        <v>5.3058</v>
-      </c>
-      <c r="D13" s="23" t="n">
-        <v>0.001599999999999518</v>
-      </c>
-      <c r="E13" s="23" t="n">
-        <v>4.830971249437988</v>
-      </c>
-      <c r="F13" s="23" t="n">
-        <v>0.05043662973838181</v>
-      </c>
-      <c r="G13" s="23" t="n">
-        <v>6.760799596175127</v>
-      </c>
-      <c r="H13" s="23" t="n">
-        <v>3.527089734383226</v>
-      </c>
-      <c r="I13" s="28" t="n">
-        <v>48936</v>
-      </c>
-      <c r="J13" s="26" t="n">
-        <v>53048.98598611611</v>
+        <v>5.1271</v>
+      </c>
+      <c r="D13" s="21" t="n">
+        <v>-0.055199999999999</v>
+      </c>
+      <c r="E13" s="21" t="n">
+        <v>4.909271586091224</v>
+      </c>
+      <c r="F13" s="21" t="n">
+        <v>-0.02576278826926792</v>
+      </c>
+      <c r="G13" s="21" t="n">
+        <v>6.563974693561869</v>
+      </c>
+      <c r="H13" s="21" t="n">
+        <v>4.123903260774209</v>
+      </c>
+      <c r="I13" s="26" t="n">
+        <v>49037</v>
+      </c>
+      <c r="J13" s="24" t="n">
+        <v>55661.9854386061</v>
       </c>
       <c r="K13" t="n">
-        <v>0.02122845481997149</v>
+        <v>0.03963634782368219</v>
       </c>
       <c r="L13" t="n">
-        <v>0.104604274412418</v>
-      </c>
-      <c r="P13" s="27">
+        <v>0.102106449606817</v>
+      </c>
+      <c r="P13" s="25">
         <f>"B"&amp;TEXT(O13,"A")</f>
         <v/>
       </c>
@@ -4271,40 +4301,40 @@
       <c r="A14" s="9" t="n">
         <v>55015</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="25" t="s">
         <v>57</v>
       </c>
       <c r="C14" s="10" t="n">
-        <v>5.29</v>
-      </c>
-      <c r="D14" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="23" t="n">
-        <v>4.855032508914769</v>
-      </c>
-      <c r="F14" s="23" t="n">
-        <v>0.05422976258220302</v>
-      </c>
-      <c r="G14" s="23" t="n">
-        <v>5.119898229615405</v>
-      </c>
-      <c r="H14" s="23" t="n">
-        <v>5.114654020371967</v>
-      </c>
-      <c r="I14" s="28" t="n">
-        <v>48936</v>
-      </c>
-      <c r="J14" s="26" t="n">
-        <v>53048.98598611611</v>
+        <v>5.1067</v>
+      </c>
+      <c r="D14" s="21" t="n">
+        <v>-0.06029999999999994</v>
+      </c>
+      <c r="E14" s="21" t="n">
+        <v>4.958046761009816</v>
+      </c>
+      <c r="F14" s="21" t="n">
+        <v>-0.02060607536156223</v>
+      </c>
+      <c r="G14" s="21" t="n">
+        <v>4.893178838738077</v>
+      </c>
+      <c r="H14" s="21" t="n">
+        <v>5.470497616377545</v>
+      </c>
+      <c r="I14" s="26" t="n">
+        <v>49037</v>
+      </c>
+      <c r="J14" s="24" t="n">
+        <v>55661.9854386061</v>
       </c>
       <c r="K14" t="n">
-        <v>0.02122845481997149</v>
+        <v>0.03963634782368219</v>
       </c>
       <c r="L14" t="n">
-        <v>0.104604274412418</v>
-      </c>
-      <c r="P14" s="27">
+        <v>0.102106449606817</v>
+      </c>
+      <c r="P14" s="25">
         <f>"B"&amp;TEXT(O14,"A")</f>
         <v/>
       </c>
@@ -4313,40 +4343,40 @@
       <c r="A15" s="9" t="n">
         <v>56749</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="25" t="s">
         <v>58</v>
       </c>
       <c r="C15" s="10" t="n">
-        <v>5.2463</v>
-      </c>
-      <c r="D15" s="23" t="n">
-        <v>0.0008999999999995123</v>
-      </c>
-      <c r="E15" s="23" t="n">
-        <v>4.904386187134513</v>
-      </c>
-      <c r="F15" s="23" t="n">
-        <v>0.05408458124287474</v>
-      </c>
-      <c r="G15" s="23" t="n">
-        <v>4.190908593593679</v>
-      </c>
-      <c r="H15" s="23" t="n">
-        <v>6.109737918972136</v>
-      </c>
-      <c r="I15" s="28" t="n">
-        <v>48936</v>
-      </c>
-      <c r="J15" s="26" t="n">
-        <v>53048.98598611611</v>
+        <v>5.06</v>
+      </c>
+      <c r="D15" s="21" t="n">
+        <v>-0.05739999999999981</v>
+      </c>
+      <c r="E15" s="21" t="n">
+        <v>5.017397134085733</v>
+      </c>
+      <c r="F15" s="21" t="n">
+        <v>-0.02363863203618255</v>
+      </c>
+      <c r="G15" s="21" t="n">
+        <v>4.014587588123231</v>
+      </c>
+      <c r="H15" s="21" t="n">
+        <v>6.361859053065322</v>
+      </c>
+      <c r="I15" s="26" t="n">
+        <v>49037</v>
+      </c>
+      <c r="J15" s="24" t="n">
+        <v>55661.9854386061</v>
       </c>
       <c r="K15" t="n">
-        <v>0.02122845481997149</v>
+        <v>0.03963634782368219</v>
       </c>
       <c r="L15" t="n">
-        <v>0.104604274412418</v>
-      </c>
-      <c r="P15" s="27">
+        <v>0.102106449606817</v>
+      </c>
+      <c r="P15" s="25">
         <f>"B"&amp;TEXT(O15,"A")</f>
         <v/>
       </c>
@@ -4371,7 +4401,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="18" min="18" style="35" width="17.5703125"/>
+    <col bestFit="1" customWidth="1" max="18" min="18" style="33" width="17.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -4416,40 +4446,40 @@
       <c r="A2" s="8" t="n">
         <v>43101</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="25" t="s">
         <v>66</v>
       </c>
       <c r="C2" t="n">
-        <v>7.7581</v>
-      </c>
-      <c r="D2" s="23" t="n">
-        <v>-0.01470000000000082</v>
-      </c>
-      <c r="E2" s="24" t="n">
-        <v>-3.189989081103933</v>
-      </c>
-      <c r="F2" s="24" t="n">
-        <v>0.02903334577530892</v>
-      </c>
-      <c r="G2" s="23" t="n">
-        <v>0.9981240658908717</v>
-      </c>
-      <c r="H2" s="25" t="n">
-        <v>8.025279003232022e-05</v>
-      </c>
-      <c r="I2" s="28" t="n">
+        <v>7.6136</v>
+      </c>
+      <c r="D2" s="21" t="n">
+        <v>-0.001700000000000312</v>
+      </c>
+      <c r="E2" s="22" t="n">
+        <v>-4.639375911146132</v>
+      </c>
+      <c r="F2" s="22" t="n">
+        <v>-0.1705347855869572</v>
+      </c>
+      <c r="G2" s="21" t="n">
+        <v>0.9949485463912212</v>
+      </c>
+      <c r="H2" s="23" t="n">
+        <v>-0.00182059812189006</v>
+      </c>
+      <c r="I2" s="26" t="n">
         <v>43102</v>
       </c>
-      <c r="J2" s="26" t="n">
-        <v>1508.704921160398</v>
-      </c>
-      <c r="K2" s="26" t="n">
-        <v>524.5014382610603</v>
+      <c r="J2" s="24" t="n">
+        <v>1437.479004234854</v>
+      </c>
+      <c r="K2" s="24" t="n">
+        <v>524.6587305281588</v>
       </c>
       <c r="L2" t="n">
-        <v>0.07773230994066882</v>
-      </c>
-      <c r="R2" s="27" t="s">
+        <v>0.07653692110022781</v>
+      </c>
+      <c r="R2" s="25" t="s">
         <v>67</v>
       </c>
     </row>
@@ -4457,40 +4487,40 @@
       <c r="A3" s="8" t="n">
         <v>43466</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="25" t="s">
         <v>68</v>
       </c>
       <c r="C3" t="n">
-        <v>7.745</v>
-      </c>
-      <c r="D3" s="23" t="n">
-        <v>0.03999999999999976</v>
-      </c>
-      <c r="E3" s="24" t="n">
-        <v>-5.499934265012079</v>
-      </c>
-      <c r="F3" s="24" t="n">
-        <v>-0.0001653724242265397</v>
-      </c>
-      <c r="G3" s="23" t="n">
-        <v>0.9946085066864554</v>
-      </c>
-      <c r="H3" s="25" t="n">
-        <v>0.0001656420168102413</v>
-      </c>
-      <c r="I3" s="28" t="n">
+        <v>7.565000000000001</v>
+      </c>
+      <c r="D3" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="22" t="n">
+        <v>-5.500040175680926</v>
+      </c>
+      <c r="F3" s="22" t="n">
+        <v>0.0001099346813582258</v>
+      </c>
+      <c r="G3" s="21" t="n">
+        <v>0.99405512144246</v>
+      </c>
+      <c r="H3" s="23" t="n">
+        <v>-0.0002401666806338687</v>
+      </c>
+      <c r="I3" s="26" t="n">
         <v>43440</v>
       </c>
-      <c r="J3" s="26" t="n">
-        <v>6023.23502366664</v>
-      </c>
-      <c r="K3" s="26" t="n">
-        <v>547.0319036352406</v>
+      <c r="J3" s="24" t="n">
+        <v>5975.940501357079</v>
+      </c>
+      <c r="K3" s="24" t="n">
+        <v>546.6707693722298</v>
       </c>
       <c r="L3" t="n">
-        <v>0.07768639773199904</v>
-      </c>
-      <c r="R3" s="27" t="s">
+        <v>0.07592490333268428</v>
+      </c>
+      <c r="R3" s="25" t="s">
         <v>67</v>
       </c>
     </row>
@@ -4498,40 +4528,40 @@
       <c r="A4" s="8" t="n">
         <v>44197</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="25" t="s">
         <v>69</v>
       </c>
       <c r="C4" t="n">
-        <v>9.064399999999999</v>
-      </c>
-      <c r="D4" s="23" t="n">
-        <v>0.03439999999999971</v>
-      </c>
-      <c r="E4" s="24" t="n">
-        <v>-14.56012840799617</v>
-      </c>
-      <c r="F4" s="24" t="n">
-        <v>0.4399882859661126</v>
-      </c>
-      <c r="G4" s="23" t="n">
-        <v>0.9962579238659411</v>
-      </c>
-      <c r="H4" s="25" t="n">
-        <v>0.0004621171637206878</v>
-      </c>
-      <c r="I4" s="28" t="n">
+        <v>8.775</v>
+      </c>
+      <c r="D4" s="21" t="n">
+        <v>-0.03769999999999885</v>
+      </c>
+      <c r="E4" s="22" t="n">
+        <v>-13.49979281122224</v>
+      </c>
+      <c r="F4" s="22" t="n">
+        <v>0.2301878859886646</v>
+      </c>
+      <c r="G4" s="21" t="n">
+        <v>0.996174961245755</v>
+      </c>
+      <c r="H4" s="23" t="n">
+        <v>-9.038200644995165e-05</v>
+      </c>
+      <c r="I4" s="26" t="n">
         <v>44035</v>
       </c>
-      <c r="J4" s="26" t="n">
-        <v>13699.65205996748</v>
-      </c>
-      <c r="K4" s="26" t="n">
-        <v>605.11543213086</v>
+      <c r="J4" s="24" t="n">
+        <v>13792.8175637847</v>
+      </c>
+      <c r="K4" s="24" t="n">
+        <v>604.153561360343</v>
       </c>
       <c r="L4" t="n">
-        <v>0.08981223700768233</v>
-      </c>
-      <c r="R4" s="27" t="s">
+        <v>0.08693718413600462</v>
+      </c>
+      <c r="R4" s="25" t="s">
         <v>67</v>
       </c>
     </row>
@@ -4539,40 +4569,40 @@
       <c r="A5" s="8" t="n">
         <v>44927</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="25" t="s">
         <v>70</v>
       </c>
       <c r="C5" t="n">
-        <v>9.613300000000001</v>
-      </c>
-      <c r="D5" s="23" t="n">
-        <v>0.02510000000000012</v>
-      </c>
-      <c r="E5" s="24" t="n">
-        <v>-22.67006526253348</v>
-      </c>
-      <c r="F5" s="24" t="n">
-        <v>0.5099422223109329</v>
-      </c>
-      <c r="G5" s="23" t="n">
-        <v>0.9942997062541229</v>
-      </c>
-      <c r="H5" s="25" t="n">
-        <v>0.0003904913706479496</v>
-      </c>
-      <c r="I5" s="28" t="n">
-        <v>44525</v>
-      </c>
-      <c r="J5" s="26" t="n">
-        <v>19797.37959449945</v>
-      </c>
-      <c r="K5" s="26" t="n">
-        <v>674.6381244387162</v>
+        <v>9.3087</v>
+      </c>
+      <c r="D5" s="21" t="n">
+        <v>-0.04409999999999969</v>
+      </c>
+      <c r="E5" s="22" t="n">
+        <v>-21.13003870687275</v>
+      </c>
+      <c r="F5" s="22" t="n">
+        <v>0.5898251973870927</v>
+      </c>
+      <c r="G5" s="21" t="n">
+        <v>0.9944367467587139</v>
+      </c>
+      <c r="H5" s="23" t="n">
+        <v>0.0001751350829239939</v>
+      </c>
+      <c r="I5" s="26" t="n">
+        <v>44529</v>
+      </c>
+      <c r="J5" s="24" t="n">
+        <v>20075.33696892217</v>
+      </c>
+      <c r="K5" s="24" t="n">
+        <v>672.7126260290698</v>
       </c>
       <c r="L5" t="n">
-        <v>0.09588726919370599</v>
-      </c>
-      <c r="R5" s="27" t="s">
+        <v>0.09289432761378065</v>
+      </c>
+      <c r="R5" s="25" t="s">
         <v>67</v>
       </c>
     </row>
@@ -4580,40 +4610,40 @@
       <c r="A6" s="8" t="n">
         <v>45658</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="25" t="s">
         <v>71</v>
       </c>
       <c r="C6" t="n">
-        <v>9.859999999999999</v>
-      </c>
-      <c r="D6" s="23" t="n">
-        <v>0.03689999999999943</v>
-      </c>
-      <c r="E6" s="24" t="n">
-        <v>-30.99996636973829</v>
-      </c>
-      <c r="F6" s="24" t="n">
-        <v>0.6899419678722829</v>
-      </c>
-      <c r="G6" s="23" t="n">
-        <v>0.9906862767093164</v>
-      </c>
-      <c r="H6" s="25" t="n">
-        <v>0.0008370630658849354</v>
-      </c>
-      <c r="I6" s="28" t="n">
-        <v>44925</v>
-      </c>
-      <c r="J6" s="26" t="n">
-        <v>24735.89568290357</v>
-      </c>
-      <c r="K6" s="26" t="n">
-        <v>757.1648615797296</v>
+        <v>9.5284</v>
+      </c>
+      <c r="D6" s="21" t="n">
+        <v>-0.06430000000000186</v>
+      </c>
+      <c r="E6" s="22" t="n">
+        <v>-29.16011912964242</v>
+      </c>
+      <c r="F6" s="22" t="n">
+        <v>0.5698843877614799</v>
+      </c>
+      <c r="G6" s="21" t="n">
+        <v>0.9904288577585045</v>
+      </c>
+      <c r="H6" s="23" t="n">
+        <v>-0.0003083580518976614</v>
+      </c>
+      <c r="I6" s="26" t="n">
+        <v>44931</v>
+      </c>
+      <c r="J6" s="24" t="n">
+        <v>25261.25048251671</v>
+      </c>
+      <c r="K6" s="24" t="n">
+        <v>753.6381515239896</v>
       </c>
       <c r="L6" t="n">
-        <v>0.09839382240325362</v>
-      </c>
-      <c r="R6" s="27" t="s">
+        <v>0.09522250959656119</v>
+      </c>
+      <c r="R6" s="25" t="s">
         <v>67</v>
       </c>
     </row>
@@ -4621,40 +4651,40 @@
       <c r="A7" s="8" t="n">
         <v>46388</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="25" t="s">
         <v>72</v>
       </c>
       <c r="C7" t="n">
-        <v>10.015</v>
-      </c>
-      <c r="D7" s="23" t="n">
-        <v>0.03790000000000043</v>
-      </c>
-      <c r="E7" s="24" t="n">
-        <v>-34.49985910966194</v>
-      </c>
-      <c r="F7" s="24" t="n">
-        <v>0.7902308204497928</v>
-      </c>
-      <c r="G7" s="23" t="n">
-        <v>0.9903699133346126</v>
-      </c>
-      <c r="H7" s="25" t="n">
-        <v>0.0009347933085718241</v>
-      </c>
-      <c r="I7" s="28" t="n">
-        <v>45258</v>
-      </c>
-      <c r="J7" s="26" t="n">
-        <v>28693.4224855262</v>
-      </c>
-      <c r="K7" s="26" t="n">
-        <v>851.7373679014563</v>
+        <v>9.705</v>
+      </c>
+      <c r="D7" s="21" t="n">
+        <v>-0.0787999999999997</v>
+      </c>
+      <c r="E7" s="22" t="n">
+        <v>-31.49991970527871</v>
+      </c>
+      <c r="F7" s="22" t="n">
+        <v>1.120132213987684</v>
+      </c>
+      <c r="G7" s="21" t="n">
+        <v>0.9916527669337725</v>
+      </c>
+      <c r="H7" s="23" t="n">
+        <v>-0.0003296485363333268</v>
+      </c>
+      <c r="I7" s="26" t="n">
+        <v>45268</v>
+      </c>
+      <c r="J7" s="24" t="n">
+        <v>29394.90131383393</v>
+      </c>
+      <c r="K7" s="24" t="n">
+        <v>845.4679517289368</v>
       </c>
       <c r="L7" t="n">
-        <v>0.1000917213947563</v>
-      </c>
-      <c r="R7" s="27" t="s">
+        <v>0.09669803574477966</v>
+      </c>
+      <c r="R7" s="25" t="s">
         <v>67</v>
       </c>
     </row>
@@ -4673,7 +4703,7 @@
   <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="C2" sqref="C2:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -4720,40 +4750,40 @@
       <c r="A2" s="8" t="n">
         <v>43009</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="28" t="s">
         <v>75</v>
       </c>
       <c r="C2" t="n">
-        <v>8.405799999999999</v>
-      </c>
-      <c r="D2" s="23" t="n">
-        <v>-0.03200000000000008</v>
-      </c>
-      <c r="E2" s="24" t="n">
-        <v>3.586571291074592</v>
-      </c>
-      <c r="F2" s="24" t="n">
-        <v>0.009135766646378496</v>
-      </c>
-      <c r="G2" s="23" t="n">
-        <v>1.008795218079044</v>
-      </c>
-      <c r="H2" s="25" t="n">
-        <v>0.0004640627036547329</v>
-      </c>
-      <c r="I2" s="28" t="n">
+        <v>8.180400000000001</v>
+      </c>
+      <c r="D2" s="21" t="n">
+        <v>-0.05529999999999979</v>
+      </c>
+      <c r="E2" s="22" t="n">
+        <v>3.841978396885853</v>
+      </c>
+      <c r="F2" s="22" t="n">
+        <v>0.07542159487422495</v>
+      </c>
+      <c r="G2" s="21" t="n">
+        <v>1.004523007383135</v>
+      </c>
+      <c r="H2" s="23" t="n">
+        <v>0.0005323025229337919</v>
+      </c>
+      <c r="I2" s="26" t="n">
         <v>43010</v>
       </c>
-      <c r="J2" s="26" t="n">
-        <v>327.5561062910128</v>
+      <c r="J2" s="24" t="n">
+        <v>255.6535184739914</v>
       </c>
       <c r="K2" t="n">
         <v>500</v>
       </c>
       <c r="L2" t="n">
-        <v>0.08329555358914775</v>
-      </c>
-      <c r="R2" s="27" t="s">
+        <v>0.08142112231722454</v>
+      </c>
+      <c r="R2" s="34" t="s">
         <v>76</v>
       </c>
     </row>
@@ -4761,40 +4791,40 @@
       <c r="A3" s="8" t="n">
         <v>43101</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="28" t="s">
         <v>77</v>
       </c>
       <c r="C3" t="n">
-        <v>7.7339</v>
-      </c>
-      <c r="D3" s="23" t="n">
-        <v>-0.01499999999999974</v>
-      </c>
-      <c r="E3" s="24" t="n">
-        <v>-5.609989081103856</v>
-      </c>
-      <c r="F3" s="24" t="n">
-        <v>-0.0009666542245829746</v>
-      </c>
-      <c r="G3" s="23" t="n">
-        <v>0.9951233369784717</v>
-      </c>
-      <c r="H3" s="25" t="n">
-        <v>3.706797143043783e-05</v>
-      </c>
-      <c r="I3" s="28" t="n">
+        <v>7.589899999999999</v>
+      </c>
+      <c r="D3" s="21" t="n">
+        <v>-0.001500000000000112</v>
+      </c>
+      <c r="E3" s="22" t="n">
+        <v>-7.009375911146143</v>
+      </c>
+      <c r="F3" s="22" t="n">
+        <v>-0.1505347855869363</v>
+      </c>
+      <c r="G3" s="21" t="n">
+        <v>0.9919615618323225</v>
+      </c>
+      <c r="H3" s="23" t="n">
+        <v>-0.0001795181569426152</v>
+      </c>
+      <c r="I3" s="26" t="n">
         <v>43102</v>
       </c>
-      <c r="J3" s="26" t="n">
-        <v>1421.353031484614</v>
+      <c r="J3" s="24" t="n">
+        <v>1353.329099645634</v>
       </c>
       <c r="K3" t="n">
         <v>500</v>
       </c>
       <c r="L3" t="n">
-        <v>0.07773230994066882</v>
-      </c>
-      <c r="R3" s="27" t="s">
+        <v>0.07653692110022781</v>
+      </c>
+      <c r="R3" s="25" t="s">
         <v>76</v>
       </c>
     </row>
@@ -4802,40 +4832,40 @@
       <c r="A4" s="8" t="n">
         <v>43191</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="28" t="s">
         <v>78</v>
       </c>
       <c r="C4" t="n">
-        <v>7.575</v>
-      </c>
-      <c r="D4" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="24" t="n">
-        <v>1.500662571503192</v>
-      </c>
-      <c r="F4" s="24" t="n">
-        <v>0.001487691325685603</v>
-      </c>
-      <c r="G4" s="23" t="n">
-        <v>1.003338604365187</v>
-      </c>
-      <c r="H4" s="25" t="n">
-        <v>1.196331441954968e-05</v>
-      </c>
-      <c r="I4" s="28" t="n">
+        <v>7.41</v>
+      </c>
+      <c r="D4" s="21" t="n">
+        <v>-0.0450000000000006</v>
+      </c>
+      <c r="E4" s="22" t="n">
+        <v>0.9998539224381764</v>
+      </c>
+      <c r="F4" s="22" t="n">
+        <v>-0.5007519817973316</v>
+      </c>
+      <c r="G4" s="21" t="n">
+        <v>1.002007749109856</v>
+      </c>
+      <c r="H4" s="23" t="n">
+        <v>-0.0005962358015960678</v>
+      </c>
+      <c r="I4" s="26" t="n">
         <v>43192</v>
       </c>
-      <c r="J4" s="26" t="n">
-        <v>2479.526348535728</v>
+      <c r="J4" s="24" t="n">
+        <v>2417.182082212094</v>
       </c>
       <c r="K4" t="n">
         <v>500</v>
       </c>
       <c r="L4" t="n">
-        <v>0.07548869734975505</v>
-      </c>
-      <c r="R4" s="27" t="s">
+        <v>0.07394618669750219</v>
+      </c>
+      <c r="R4" s="25" t="s">
         <v>76</v>
       </c>
     </row>
@@ -4843,40 +4873,40 @@
       <c r="A5" s="8" t="n">
         <v>43282</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="28" t="s">
         <v>79</v>
       </c>
       <c r="C5" t="n">
-        <v>7.568900000000001</v>
-      </c>
-      <c r="D5" s="23" t="n">
-        <v>0.02140000000000059</v>
-      </c>
-      <c r="E5" s="24" t="n">
-        <v>1.389356486983795</v>
-      </c>
-      <c r="F5" s="24" t="n">
-        <v>0.1399308962309054</v>
-      </c>
-      <c r="G5" s="23" t="n">
-        <v>1.002761225523287</v>
-      </c>
-      <c r="H5" s="25" t="n">
-        <v>0.0001641966198360212</v>
-      </c>
-      <c r="I5" s="28" t="n">
+        <v>7.3879</v>
+      </c>
+      <c r="D5" s="21" t="n">
+        <v>-0.05210000000000076</v>
+      </c>
+      <c r="E5" s="22" t="n">
+        <v>0.7903943256157286</v>
+      </c>
+      <c r="F5" s="22" t="n">
+        <v>-0.7097711372840154</v>
+      </c>
+      <c r="G5" s="21" t="n">
+        <v>1.001529944467866</v>
+      </c>
+      <c r="H5" s="23" t="n">
+        <v>-0.0008819431342281803</v>
+      </c>
+      <c r="I5" s="26" t="n">
         <v>43283</v>
       </c>
-      <c r="J5" s="26" t="n">
-        <v>3530.639353499282</v>
+      <c r="J5" s="24" t="n">
+        <v>3475.540024297516</v>
       </c>
       <c r="K5" t="n">
         <v>500</v>
       </c>
       <c r="L5" t="n">
-        <v>0.07547293827600177</v>
-      </c>
-      <c r="R5" s="27" t="s">
+        <v>0.07376209488384222</v>
+      </c>
+      <c r="R5" s="25" t="s">
         <v>76</v>
       </c>
     </row>
@@ -4884,40 +4914,40 @@
       <c r="A6" s="8" t="n">
         <v>43374</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="28" t="s">
         <v>80</v>
       </c>
       <c r="C6" t="n">
-        <v>7.664999999999999</v>
-      </c>
-      <c r="D6" s="23" t="n">
-        <v>0.03999999999999976</v>
-      </c>
-      <c r="E6" s="24" t="n">
-        <v>1.500186029240735</v>
-      </c>
-      <c r="F6" s="24" t="n">
-        <v>-0.0002322603305515702</v>
-      </c>
-      <c r="G6" s="23" t="n">
-        <v>1.002588356130373</v>
-      </c>
-      <c r="H6" s="25" t="n">
-        <v>-3.041966897487924e-05</v>
-      </c>
-      <c r="I6" s="28" t="n">
+        <v>7.470000000000001</v>
+      </c>
+      <c r="D6" s="21" t="n">
+        <v>-0.04499999999999921</v>
+      </c>
+      <c r="E6" s="22" t="n">
+        <v>1.000454708530857</v>
+      </c>
+      <c r="F6" s="22" t="n">
+        <v>-0.5000454511343289</v>
+      </c>
+      <c r="G6" s="21" t="n">
+        <v>1.001626797296712</v>
+      </c>
+      <c r="H6" s="23" t="n">
+        <v>-0.0006138461403153439</v>
+      </c>
+      <c r="I6" s="26" t="n">
         <v>43374</v>
       </c>
-      <c r="J6" s="26" t="n">
-        <v>4565.819021117932</v>
+      <c r="J6" s="24" t="n">
+        <v>4519.693949241628</v>
       </c>
       <c r="K6" t="n">
         <v>500</v>
       </c>
       <c r="L6" t="n">
-        <v>0.07644476697916969</v>
-      </c>
-      <c r="R6" s="27" t="s">
+        <v>0.0745742782429617</v>
+      </c>
+      <c r="R6" s="25" t="s">
         <v>76</v>
       </c>
     </row>
@@ -4925,40 +4955,40 @@
       <c r="A7" s="8" t="n">
         <v>43466</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="28" t="s">
         <v>81</v>
       </c>
       <c r="C7" t="n">
-        <v>7.8083</v>
-      </c>
-      <c r="D7" s="23" t="n">
-        <v>0.03830000000000083</v>
-      </c>
-      <c r="E7" s="24" t="n">
-        <v>0.8300657349878671</v>
-      </c>
-      <c r="F7" s="24" t="n">
-        <v>-0.1701653724241192</v>
-      </c>
-      <c r="G7" s="23" t="n">
-        <v>1.001524582109143</v>
-      </c>
-      <c r="H7" s="25" t="n">
-        <v>-0.0002328894830285755</v>
-      </c>
-      <c r="I7" s="28" t="n">
+        <v>7.6279</v>
+      </c>
+      <c r="D7" s="21" t="n">
+        <v>-0.001500000000000112</v>
+      </c>
+      <c r="E7" s="22" t="n">
+        <v>0.7899598243189809</v>
+      </c>
+      <c r="F7" s="22" t="n">
+        <v>-0.149890065318653</v>
+      </c>
+      <c r="G7" s="21" t="n">
+        <v>1.001201264463147</v>
+      </c>
+      <c r="H7" s="23" t="n">
+        <v>-0.0001890902571155539</v>
+      </c>
+      <c r="I7" s="26" t="n">
         <v>43467</v>
       </c>
-      <c r="J7" s="26" t="n">
-        <v>5488.882198987994</v>
+      <c r="J7" s="24" t="n">
+        <v>5449.479456623521</v>
       </c>
       <c r="K7" t="n">
         <v>500</v>
       </c>
       <c r="L7" t="n">
-        <v>0.07795963840480158</v>
-      </c>
-      <c r="R7" s="27" t="s">
+        <v>0.07618409163949491</v>
+      </c>
+      <c r="R7" s="25" t="s">
         <v>76</v>
       </c>
     </row>
@@ -4966,40 +4996,40 @@
       <c r="A8" s="8" t="n">
         <v>43556</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="28" t="s">
         <v>82</v>
       </c>
       <c r="C8" t="n">
-        <v>7.985</v>
-      </c>
-      <c r="D8" s="23" t="n">
-        <v>0.03999999999999976</v>
-      </c>
-      <c r="E8" s="24" t="n">
-        <v>1.500022561143066</v>
-      </c>
-      <c r="F8" s="24" t="n">
-        <v>0.0003272485464556052</v>
-      </c>
-      <c r="G8" s="23" t="n">
-        <v>1.002172189981834</v>
-      </c>
-      <c r="H8" s="25" t="n">
-        <v>-2.232123949297282e-05</v>
-      </c>
-      <c r="I8" s="28" t="n">
+        <v>7.765</v>
+      </c>
+      <c r="D8" s="21" t="n">
+        <v>-0.02000000000000057</v>
+      </c>
+      <c r="E8" s="22" t="n">
+        <v>1.50003745939653</v>
+      </c>
+      <c r="F8" s="22" t="n">
+        <v>9.674636175516227e-05</v>
+      </c>
+      <c r="G8" s="21" t="n">
+        <v>1.001990545465363</v>
+      </c>
+      <c r="H8" s="23" t="n">
+        <v>1.213202133354407e-05</v>
+      </c>
+      <c r="I8" s="26" t="n">
         <v>43556</v>
       </c>
-      <c r="J8" s="26" t="n">
-        <v>6377.001447479415</v>
+      <c r="J8" s="24" t="n">
+        <v>6352.229523909045</v>
       </c>
       <c r="K8" t="n">
         <v>500</v>
       </c>
       <c r="L8" t="n">
-        <v>0.07967023584233335</v>
-      </c>
-      <c r="R8" s="27" t="s">
+        <v>0.0774899369658415</v>
+      </c>
+      <c r="R8" s="25" t="s">
         <v>76</v>
       </c>
     </row>
@@ -5007,40 +5037,40 @@
       <c r="A9" s="8" t="n">
         <v>43647</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="28" t="s">
         <v>83</v>
       </c>
       <c r="C9" t="n">
-        <v>8.17</v>
-      </c>
-      <c r="D9" s="23" t="n">
-        <v>0.01999999999999919</v>
-      </c>
-      <c r="E9" s="24" t="n">
-        <v>0.9997202244560466</v>
-      </c>
-      <c r="F9" s="24" t="n">
-        <v>-0.0004028841925352022</v>
-      </c>
-      <c r="G9" s="23" t="n">
-        <v>1.001432696874223</v>
-      </c>
-      <c r="H9" s="25" t="n">
-        <v>-8.735706877649463e-06</v>
-      </c>
-      <c r="I9" s="28" t="n">
+        <v>7.9516</v>
+      </c>
+      <c r="D9" s="21" t="n">
+        <v>-0.01839999999999897</v>
+      </c>
+      <c r="E9" s="22" t="n">
+        <v>1.159782752163385</v>
+      </c>
+      <c r="F9" s="22" t="n">
+        <v>0.1597394267680019</v>
+      </c>
+      <c r="G9" s="21" t="n">
+        <v>1.001460460403481</v>
+      </c>
+      <c r="H9" s="23" t="n">
+        <v>0.0002025000488581341</v>
+      </c>
+      <c r="I9" s="26" t="n">
         <v>43647</v>
       </c>
-      <c r="J9" s="26" t="n">
-        <v>7215.22295635441</v>
+      <c r="J9" s="24" t="n">
+        <v>7200.803166368132</v>
       </c>
       <c r="K9" t="n">
         <v>500</v>
       </c>
       <c r="L9" t="n">
-        <v>0.08157849211810775</v>
-      </c>
-      <c r="R9" s="27" t="s">
+        <v>0.07939557156086186</v>
+      </c>
+      <c r="R9" s="25" t="s">
         <v>76</v>
       </c>
     </row>
@@ -5048,40 +5078,40 @@
       <c r="A10" s="8" t="n">
         <v>43739</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="28" t="s">
         <v>84</v>
       </c>
       <c r="C10" t="n">
-        <v>8.41</v>
-      </c>
-      <c r="D10" s="23" t="n">
-        <v>0.008900000000000574</v>
-      </c>
-      <c r="E10" s="24" t="n">
-        <v>2.000002538879442</v>
-      </c>
-      <c r="F10" s="24" t="n">
-        <v>-0.1099724477571229</v>
-      </c>
-      <c r="G10" s="23" t="n">
-        <v>1.002455795732486</v>
-      </c>
-      <c r="H10" s="25" t="n">
-        <v>-0.000131027559342245</v>
-      </c>
-      <c r="I10" s="28" t="n">
+        <v>8.173299999999999</v>
+      </c>
+      <c r="D10" s="21" t="n">
+        <v>-0.04009999999999986</v>
+      </c>
+      <c r="E10" s="22" t="n">
+        <v>2.329768155521772</v>
+      </c>
+      <c r="F10" s="22" t="n">
+        <v>-0.01026328714584501</v>
+      </c>
+      <c r="G10" s="21" t="n">
+        <v>1.002747327637235</v>
+      </c>
+      <c r="H10" s="23" t="n">
+        <v>1.098949239075608e-05</v>
+      </c>
+      <c r="I10" s="26" t="n">
         <v>43739</v>
       </c>
-      <c r="J10" s="26" t="n">
-        <v>8043.430892706965</v>
+      <c r="J10" s="24" t="n">
+        <v>8045.019394554402</v>
       </c>
       <c r="K10" t="n">
         <v>500</v>
       </c>
       <c r="L10" t="n">
-        <v>0.0838855987408833</v>
-      </c>
-      <c r="R10" s="27" t="s">
+        <v>0.08150021741322266</v>
+      </c>
+      <c r="R10" s="25" t="s">
         <v>76</v>
       </c>
     </row>
@@ -5089,40 +5119,40 @@
       <c r="A11" s="8" t="n">
         <v>43831</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="28" t="s">
         <v>85</v>
       </c>
       <c r="C11" t="n">
-        <v>8.59</v>
-      </c>
-      <c r="D11" s="23" t="n">
-        <v>0.02999999999999947</v>
-      </c>
-      <c r="E11" s="24" t="n">
-        <v>0.9998319409412759</v>
-      </c>
-      <c r="F11" s="24" t="n">
-        <v>-3.787165886448562e-05</v>
-      </c>
-      <c r="G11" s="23" t="n">
-        <v>1.001226104230071</v>
-      </c>
-      <c r="H11" s="25" t="n">
-        <v>-1.007425676435858e-05</v>
-      </c>
-      <c r="I11" s="28" t="n">
+        <v>8.32</v>
+      </c>
+      <c r="D11" s="21" t="n">
+        <v>-0.03999999999999976</v>
+      </c>
+      <c r="E11" s="22" t="n">
+        <v>1.000151725079612</v>
+      </c>
+      <c r="F11" s="22" t="n">
+        <v>0.0001939923661986587</v>
+      </c>
+      <c r="G11" s="21" t="n">
+        <v>1.001122868673885</v>
+      </c>
+      <c r="H11" s="23" t="n">
+        <v>1.370765578423416e-05</v>
+      </c>
+      <c r="I11" s="26" t="n">
         <v>43832</v>
       </c>
-      <c r="J11" s="26" t="n">
-        <v>8791.139104901958</v>
+      <c r="J11" s="24" t="n">
+        <v>8814.12354636268</v>
       </c>
       <c r="K11" t="n">
         <v>500</v>
       </c>
       <c r="L11" t="n">
-        <v>0.08579043607325731</v>
-      </c>
-      <c r="R11" s="27" t="s">
+        <v>0.08310292320856738</v>
+      </c>
+      <c r="R11" s="25" t="s">
         <v>76</v>
       </c>
     </row>
@@ -5130,40 +5160,40 @@
       <c r="A12" s="8" t="n">
         <v>44013</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="28" t="s">
         <v>86</v>
       </c>
       <c r="C12" t="n">
-        <v>8.949999999999999</v>
-      </c>
-      <c r="D12" s="23" t="n">
-        <v>0.03999999999999976</v>
-      </c>
-      <c r="E12" s="24" t="n">
-        <v>0.9997973998396303</v>
-      </c>
-      <c r="F12" s="24" t="n">
-        <v>-1.467421253953383e-05</v>
-      </c>
-      <c r="G12" s="23" t="n">
-        <v>1.001102311342175</v>
-      </c>
-      <c r="H12" s="25" t="n">
-        <v>-1.121586434127408e-05</v>
-      </c>
-      <c r="I12" s="28" t="n">
+        <v>8.66</v>
+      </c>
+      <c r="D12" s="21" t="n">
+        <v>-0.03999999999999976</v>
+      </c>
+      <c r="E12" s="22" t="n">
+        <v>0.999860395525104</v>
+      </c>
+      <c r="F12" s="22" t="n">
+        <v>-7.515963892923416e-05</v>
+      </c>
+      <c r="G12" s="21" t="n">
+        <v>1.001028505687444</v>
+      </c>
+      <c r="H12" s="23" t="n">
+        <v>1.104107309735092e-05</v>
+      </c>
+      <c r="I12" s="26" t="n">
         <v>44013</v>
       </c>
-      <c r="J12" s="26" t="n">
-        <v>10112.33837749387</v>
+      <c r="J12" s="24" t="n">
+        <v>10170.84429055103</v>
       </c>
       <c r="K12" t="n">
         <v>500</v>
       </c>
       <c r="L12" t="n">
-        <v>0.08939719002835522</v>
-      </c>
-      <c r="R12" s="27" t="s">
+        <v>0.08650729606639285</v>
+      </c>
+      <c r="R12" s="25" t="s">
         <v>76</v>
       </c>
     </row>
@@ -5171,40 +5201,40 @@
       <c r="A13" s="8" t="n">
         <v>44378</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="28" t="s">
         <v>87</v>
       </c>
       <c r="C13" t="n">
-        <v>9.4564</v>
-      </c>
-      <c r="D13" s="23" t="n">
-        <v>0.01990000000000047</v>
-      </c>
-      <c r="E13" s="24" t="n">
-        <v>0.6398123236986408</v>
-      </c>
-      <c r="F13" s="24" t="n">
-        <v>-0.01032805371059542</v>
-      </c>
-      <c r="G13" s="23" t="n">
-        <v>1.000614629868937</v>
-      </c>
-      <c r="H13" s="25" t="n">
-        <v>-1.399243509236925e-05</v>
-      </c>
-      <c r="I13" s="28" t="n">
+        <v>9.160500000000001</v>
+      </c>
+      <c r="D13" s="21" t="n">
+        <v>-0.04829999999999973</v>
+      </c>
+      <c r="E13" s="22" t="n">
+        <v>1.050129212865764</v>
+      </c>
+      <c r="F13" s="22" t="n">
+        <v>0.1699409739021329</v>
+      </c>
+      <c r="G13" s="21" t="n">
+        <v>1.000987467638955</v>
+      </c>
+      <c r="H13" s="23" t="n">
+        <v>0.0001877992989836041</v>
+      </c>
+      <c r="I13" s="26" t="n">
         <v>44378</v>
       </c>
-      <c r="J13" s="26" t="n">
-        <v>12308.84437002169</v>
+      <c r="J13" s="24" t="n">
+        <v>12434.91296011416</v>
       </c>
       <c r="K13" t="n">
         <v>500</v>
       </c>
       <c r="L13" t="n">
-        <v>0.09450326267762077</v>
-      </c>
-      <c r="R13" s="27" t="s">
+        <v>0.09151063456665098</v>
+      </c>
+      <c r="R13" s="25" t="s">
         <v>76</v>
       </c>
     </row>
@@ -5222,8 +5252,8 @@
   </sheetPr>
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -5262,10 +5292,10 @@
         <v>96</v>
       </c>
       <c r="C2" t="n">
-        <v>1898675</v>
+        <v>2211302</v>
       </c>
       <c r="E2" t="n">
-        <v>6148.422040922871</v>
+        <v>7915.990700492034</v>
       </c>
       <c r="F2" t="n">
         <v>5086.04817860171</v>
@@ -5274,7 +5304,7 @@
         <v>5191.96931242336</v>
       </c>
       <c r="H2" t="n">
-        <v>4856.107068302347</v>
+        <v>4883.425365264343</v>
       </c>
       <c r="I2" t="n">
         <v>4928.287555311905</v>
@@ -5285,16 +5315,16 @@
         <v>97</v>
       </c>
       <c r="B3" t="n">
-        <v>8.369999999999999</v>
+        <v>8.141999999999999</v>
       </c>
       <c r="C3" t="n">
-        <v>380935</v>
+        <v>266325</v>
       </c>
       <c r="D3" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E3" t="n">
-        <v>88.27052913378635</v>
+        <v>50.39643017432024</v>
       </c>
       <c r="F3" t="n">
         <v>104.8748845376868</v>
@@ -5314,16 +5344,16 @@
         <v>98</v>
       </c>
       <c r="B4" t="n">
-        <v>8.19</v>
+        <v>8.07</v>
       </c>
       <c r="C4" t="n">
-        <v>23665</v>
+        <v>7260</v>
       </c>
       <c r="D4" t="n">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E4" t="n">
-        <v>11.18807957266514</v>
+        <v>3.158675769324221</v>
       </c>
       <c r="F4" t="n">
         <v>1.964883252610876</v>
@@ -5343,16 +5373,16 @@
         <v>99</v>
       </c>
       <c r="B5" t="n">
-        <v>7.95</v>
+        <v>7.835</v>
       </c>
       <c r="C5" t="n">
-        <v>12850</v>
+        <v>102270</v>
       </c>
       <c r="D5" t="n">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E5" t="n">
-        <v>9.007055076825079</v>
+        <v>68.30839091879243</v>
       </c>
       <c r="F5" t="n">
         <v>2.100666683468131</v>
@@ -5372,16 +5402,16 @@
         <v>66</v>
       </c>
       <c r="B6" t="n">
-        <v>7.79</v>
+        <v>7.66</v>
       </c>
       <c r="C6" t="n">
-        <v>420170</v>
+        <v>251850</v>
       </c>
       <c r="D6" t="n">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E6" t="n">
-        <v>389.4703747067159</v>
+        <v>226.3625306564499</v>
       </c>
       <c r="F6" t="n">
         <v>505.7848141641472</v>
@@ -5390,7 +5420,7 @@
         <v>428.3112500464898</v>
       </c>
       <c r="H6" t="n">
-        <v>380.0332644273999</v>
+        <v>377.4442510297766</v>
       </c>
       <c r="I6" t="n">
         <v>467.9650110110565</v>
@@ -5401,16 +5431,16 @@
         <v>100</v>
       </c>
       <c r="B7" t="n">
-        <v>7.68</v>
+        <v>7.527</v>
       </c>
       <c r="C7" t="n">
-        <v>2025</v>
+        <v>1330</v>
       </c>
       <c r="D7" t="n">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E7" t="n">
-        <v>2.374691158168524</v>
+        <v>1.529706275388546</v>
       </c>
       <c r="F7" t="n">
         <v>0.2332537531632742</v>
@@ -5419,7 +5449,7 @@
         <v>2.499232501093198</v>
       </c>
       <c r="H7" t="n">
-        <v>4.219715361703096</v>
+        <v>4.20630290324627</v>
       </c>
       <c r="I7" t="n">
         <v>2.091010925627987</v>
@@ -5430,16 +5460,16 @@
         <v>101</v>
       </c>
       <c r="B8" t="n">
-        <v>7.614</v>
+        <v>7.469</v>
       </c>
       <c r="C8" t="n">
-        <v>4065</v>
+        <v>1230</v>
       </c>
       <c r="D8" t="n">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E8" t="n">
-        <v>5.575573797724956</v>
+        <v>1.664577605367097</v>
       </c>
       <c r="F8" t="n">
         <v>1.462841335374022</v>
@@ -5448,7 +5478,7 @@
         <v>2.041652460863693</v>
       </c>
       <c r="H8" t="n">
-        <v>1.024077245080173</v>
+        <v>0.9619979404395718</v>
       </c>
       <c r="I8" t="n">
         <v>0.4677880368438565</v>
@@ -5459,16 +5489,16 @@
         <v>102</v>
       </c>
       <c r="B9" t="n">
-        <v>7.56</v>
+        <v>7.4</v>
       </c>
       <c r="C9" t="n">
-        <v>58220</v>
+        <v>84457</v>
       </c>
       <c r="D9" t="n">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E9" t="n">
-        <v>93.21574480792397</v>
+        <v>134.1382232582858</v>
       </c>
       <c r="F9" t="n">
         <v>47.32163781121359</v>
@@ -5488,16 +5518,16 @@
         <v>103</v>
       </c>
       <c r="B10" t="n">
-        <v>7.555</v>
+        <v>7.38</v>
       </c>
       <c r="C10" t="n">
-        <v>109320</v>
+        <v>145415</v>
       </c>
       <c r="D10" t="n">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E10" t="n">
-        <v>248.1453420142191</v>
+        <v>330.5501832955226</v>
       </c>
       <c r="F10" t="n">
         <v>157.7256968100318</v>
@@ -5517,16 +5547,16 @@
         <v>104</v>
       </c>
       <c r="B11" t="n">
-        <v>7.65</v>
+        <v>7.46</v>
       </c>
       <c r="C11" t="n">
-        <v>11955</v>
+        <v>31140</v>
       </c>
       <c r="D11" t="n">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="E11" t="n">
-        <v>34.89222061249703</v>
+        <v>91.51230616304747</v>
       </c>
       <c r="F11" t="n">
         <v>12.29256872131019</v>
@@ -5546,16 +5576,16 @@
         <v>68</v>
       </c>
       <c r="B12" t="n">
-        <v>7.8</v>
+        <v>7.62</v>
       </c>
       <c r="C12" t="n">
-        <v>290415</v>
+        <v>701075</v>
       </c>
       <c r="D12" t="n">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="E12" t="n">
-        <v>1020.935460902979</v>
+        <v>2489.172121598707</v>
       </c>
       <c r="F12" t="n">
         <v>912.2071308307015</v>
@@ -5575,16 +5605,16 @@
         <v>105</v>
       </c>
       <c r="B13" t="n">
-        <v>7.97</v>
+        <v>7.75</v>
       </c>
       <c r="C13" t="n">
-        <v>4240</v>
+        <v>6580</v>
       </c>
       <c r="D13" t="n">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E13" t="n">
-        <v>17.26467844655938</v>
+        <v>27.14867597007378</v>
       </c>
       <c r="F13" t="n">
         <v>60.69419523453431</v>
@@ -5604,16 +5634,16 @@
         <v>106</v>
       </c>
       <c r="B14" t="n">
-        <v>8.16</v>
+        <v>7.94</v>
       </c>
       <c r="C14" t="n">
-        <v>41870</v>
+        <v>16120</v>
       </c>
       <c r="D14" t="n">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="E14" t="n">
-        <v>192.8113239299007</v>
+        <v>75.36356950939434</v>
       </c>
       <c r="F14" t="n">
         <v>61.63571112920621</v>
@@ -5633,16 +5663,16 @@
         <v>107</v>
       </c>
       <c r="B15" t="n">
-        <v>8.390000000000001</v>
+        <v>8.15</v>
       </c>
       <c r="C15" t="n">
-        <v>11980</v>
+        <v>18950</v>
       </c>
       <c r="D15" t="n">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="E15" t="n">
-        <v>61.50146676199569</v>
+        <v>98.98734316532871</v>
       </c>
       <c r="F15" t="n">
         <v>3.684319203518196</v>
@@ -5662,16 +5692,16 @@
         <v>108</v>
       </c>
       <c r="B16" t="n">
-        <v>8.58</v>
+        <v>8.31</v>
       </c>
       <c r="C16" t="n">
-        <v>139645</v>
+        <v>217670</v>
       </c>
       <c r="D16" t="n">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="E16" t="n">
-        <v>784.2491743361004</v>
+        <v>1246.768847432263</v>
       </c>
       <c r="F16" t="n">
         <v>524.0706347352395</v>
@@ -5691,16 +5721,16 @@
         <v>109</v>
       </c>
       <c r="B17" t="n">
-        <v>8.755000000000001</v>
+        <v>8.48</v>
       </c>
       <c r="C17" t="n">
-        <v>1140</v>
+        <v>560</v>
       </c>
       <c r="D17" t="n">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="E17" t="n">
-        <v>6.900257825063585</v>
+        <v>3.462075268163916</v>
       </c>
       <c r="F17" t="n">
         <v>4.136283406663354</v>
@@ -5720,16 +5750,16 @@
         <v>110</v>
       </c>
       <c r="B18" t="n">
-        <v>8.94</v>
+        <v>8.65</v>
       </c>
       <c r="C18" t="n">
-        <v>44250</v>
+        <v>19075</v>
       </c>
       <c r="D18" t="n">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E18" t="n">
-        <v>285.3833189777877</v>
+        <v>125.8633445156115</v>
       </c>
       <c r="F18" t="n">
         <v>218.9021266174602</v>
@@ -5749,16 +5779,16 @@
         <v>111</v>
       </c>
       <c r="B19" t="n">
-        <v>9.095000000000001</v>
+        <v>8.815</v>
       </c>
       <c r="C19" t="n">
-        <v>1525</v>
+        <v>600</v>
       </c>
       <c r="D19" t="n">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="E19" t="n">
-        <v>10.44436288595276</v>
+        <v>4.207566217577601</v>
       </c>
       <c r="F19" t="n">
         <v>0.5224525299891731</v>
@@ -5778,16 +5808,16 @@
         <v>69</v>
       </c>
       <c r="B20" t="n">
-        <v>9.210000000000001</v>
+        <v>8.91</v>
       </c>
       <c r="C20" t="n">
-        <v>171005</v>
+        <v>164795</v>
       </c>
       <c r="D20" t="n">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="E20" t="n">
-        <v>1233.858051541385</v>
+        <v>1219.726871369236</v>
       </c>
       <c r="F20" t="n">
         <v>1190.296562244001</v>
@@ -5807,16 +5837,16 @@
         <v>112</v>
       </c>
       <c r="B21" t="n">
-        <v>9.324999999999999</v>
+        <v>9.025</v>
       </c>
       <c r="C21" t="n">
-        <v>565</v>
+        <v>120</v>
       </c>
       <c r="D21" t="n">
-        <v>896</v>
+        <v>892</v>
       </c>
       <c r="E21" t="n">
-        <v>4.261693319083611</v>
+        <v>0.9294160804200531</v>
       </c>
       <c r="F21" t="n">
         <v>0.1182697793451248</v>
@@ -5836,16 +5866,16 @@
         <v>113</v>
       </c>
       <c r="B22" t="n">
-        <v>9.449999999999999</v>
+        <v>9.15</v>
       </c>
       <c r="C22" t="n">
-        <v>22930</v>
+        <v>30150</v>
       </c>
       <c r="D22" t="n">
-        <v>958</v>
+        <v>954</v>
       </c>
       <c r="E22" t="n">
-        <v>179.9227778414783</v>
+        <v>243.1563291541003</v>
       </c>
       <c r="F22" t="n">
         <v>8.570461171192701</v>
@@ -5865,16 +5895,16 @@
         <v>114</v>
       </c>
       <c r="B23" t="n">
-        <v>9.550000000000001</v>
+        <v>9.23</v>
       </c>
       <c r="C23" t="n">
-        <v>45</v>
+        <v>175</v>
       </c>
       <c r="D23" t="n">
-        <v>1023</v>
+        <v>1019</v>
       </c>
       <c r="E23" t="n">
-        <v>0.366676322595001</v>
+        <v>1.468417505997387</v>
       </c>
       <c r="F23" t="n">
         <v>0.09292795156538433</v>
@@ -5894,16 +5924,16 @@
         <v>115</v>
       </c>
       <c r="B24" t="n">
-        <v>9.609999999999999</v>
+        <v>9.32</v>
       </c>
       <c r="C24" t="n">
-        <v>4400</v>
+        <v>12675</v>
       </c>
       <c r="D24" t="n">
-        <v>1086</v>
+        <v>1082</v>
       </c>
       <c r="E24" t="n">
-        <v>37.09467281821502</v>
+        <v>109.9850319070107</v>
       </c>
       <c r="F24" t="n">
         <v>45.51313681076557</v>
@@ -5923,16 +5953,16 @@
         <v>116</v>
       </c>
       <c r="B25" t="n">
-        <v>9.744999999999999</v>
+        <v>9.425000000000001</v>
       </c>
       <c r="C25" t="n">
-        <v>180</v>
+        <v>5</v>
       </c>
       <c r="D25" t="n">
-        <v>1210</v>
+        <v>1206</v>
       </c>
       <c r="E25" t="n">
-        <v>1.604636912875215</v>
+        <v>0.04602785639571307</v>
       </c>
       <c r="F25" t="n">
         <v>0.09194657402897673</v>
@@ -5952,16 +5982,16 @@
         <v>70</v>
       </c>
       <c r="B26" t="n">
-        <v>9.84</v>
+        <v>9.52</v>
       </c>
       <c r="C26" t="n">
-        <v>52185</v>
+        <v>63715</v>
       </c>
       <c r="D26" t="n">
-        <v>1337</v>
+        <v>1333</v>
       </c>
       <c r="E26" t="n">
-        <v>487.8360193058793</v>
+        <v>616.1569073938452</v>
       </c>
       <c r="F26" t="n">
         <v>460.9194217210015</v>
@@ -5981,13 +6011,13 @@
         <v>117</v>
       </c>
       <c r="B27" t="n">
-        <v>9.922000000000001</v>
+        <v>9.589</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>1461</v>
+        <v>1457</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
@@ -6010,16 +6040,16 @@
         <v>118</v>
       </c>
       <c r="B28" t="n">
-        <v>10.026</v>
+        <v>9.68</v>
       </c>
       <c r="C28" t="n">
-        <v>45</v>
+        <v>475</v>
       </c>
       <c r="D28" t="n">
-        <v>1586</v>
+        <v>1582</v>
       </c>
       <c r="E28" t="n">
-        <v>0.4492393780741463</v>
+        <v>4.930399915243862</v>
       </c>
       <c r="F28" t="n">
         <v>6.809917289472142</v>
@@ -6039,13 +6069,13 @@
         <v>119</v>
       </c>
       <c r="B29" t="n">
-        <v>10.09</v>
+        <v>9.742000000000001</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>1710</v>
+        <v>1706</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
@@ -6068,16 +6098,16 @@
         <v>71</v>
       </c>
       <c r="B30" t="n">
-        <v>10.17</v>
+        <v>9.82</v>
       </c>
       <c r="C30" t="n">
-        <v>42760</v>
+        <v>41340</v>
       </c>
       <c r="D30" t="n">
-        <v>1840</v>
+        <v>1836</v>
       </c>
       <c r="E30" t="n">
-        <v>444.9154514639586</v>
+        <v>448.9407608444234</v>
       </c>
       <c r="F30" t="n">
         <v>315.8853773332613</v>
@@ -6097,16 +6127,16 @@
         <v>120</v>
       </c>
       <c r="B31" t="n">
-        <v>10.255</v>
+        <v>9.914999999999999</v>
       </c>
       <c r="C31" t="n">
-        <v>1920</v>
+        <v>1460</v>
       </c>
       <c r="D31" t="n">
-        <v>2093</v>
+        <v>2089</v>
       </c>
       <c r="E31" t="n">
-        <v>20.47129554343645</v>
+        <v>16.28942729039825</v>
       </c>
       <c r="F31" t="n">
         <v>0.7853746341039872</v>
@@ -6126,16 +6156,16 @@
         <v>72</v>
       </c>
       <c r="B32" t="n">
-        <v>10.36</v>
+        <v>10.02</v>
       </c>
       <c r="C32" t="n">
-        <v>44370</v>
+        <v>24170</v>
       </c>
       <c r="D32" t="n">
-        <v>2343</v>
+        <v>2339</v>
       </c>
       <c r="E32" t="n">
-        <v>476.0118715290259</v>
+        <v>272.2241757873098</v>
       </c>
       <c r="F32" t="n">
         <v>263.4994746808906</v>
@@ -6155,13 +6185,13 @@
         <v>121</v>
       </c>
       <c r="B33" t="n">
-        <v>10.396</v>
+        <v>10.056</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>2594</v>
+        <v>2590</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
@@ -6184,16 +6214,16 @@
         <v>122</v>
       </c>
       <c r="B34" t="n">
-        <v>10.412</v>
+        <v>10.072</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>315</v>
       </c>
       <c r="D34" t="n">
-        <v>2843</v>
+        <v>2839</v>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>3.542367594033517</v>
       </c>
       <c r="F34" t="n">
         <v>0</v>
@@ -6213,13 +6243,13 @@
         <v>123</v>
       </c>
       <c r="B35" t="n">
-        <v>10.45</v>
+        <v>10.11</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>3093</v>
+        <v>3089</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
@@ -6288,28 +6318,28 @@
         <v>132</v>
       </c>
       <c r="B2" t="n">
-        <v>6042192</v>
+        <v>5814632</v>
       </c>
       <c r="C2" t="n">
-        <v>27.36</v>
+        <v>26.23</v>
       </c>
       <c r="D2" t="n">
-        <v>37680</v>
+        <v>-325845</v>
       </c>
       <c r="E2" t="n">
-        <v>6772132</v>
+        <v>6900828</v>
       </c>
       <c r="F2" t="n">
-        <v>30.67</v>
+        <v>31.14</v>
       </c>
       <c r="G2" t="n">
-        <v>-173967</v>
+        <v>111941</v>
       </c>
       <c r="H2" t="n">
-        <v>-729940</v>
+        <v>-1086196</v>
       </c>
       <c r="I2" t="n">
-        <v>211647</v>
+        <v>-437786</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -6317,28 +6347,28 @@
         <v>133</v>
       </c>
       <c r="B3" t="n">
-        <v>6031482</v>
+        <v>5803922</v>
       </c>
       <c r="C3" t="n">
-        <v>27.31</v>
+        <v>26.19</v>
       </c>
       <c r="D3" t="n">
-        <v>40190</v>
+        <v>-325845</v>
       </c>
       <c r="E3" t="n">
-        <v>6597317</v>
+        <v>6726378</v>
       </c>
       <c r="F3" t="n">
-        <v>29.87</v>
+        <v>30.35</v>
       </c>
       <c r="G3" t="n">
-        <v>-173312</v>
+        <v>111446</v>
       </c>
       <c r="H3" t="n">
-        <v>-565835</v>
+        <v>-922456</v>
       </c>
       <c r="I3" t="n">
-        <v>213502</v>
+        <v>-437291</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -6361,13 +6391,13 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>-200</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
         <v>-1920</v>
       </c>
       <c r="I4" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -6381,22 +6411,22 @@
         <v>0.04</v>
       </c>
       <c r="D5" t="n">
-        <v>-2510</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>172895</v>
+        <v>172530</v>
       </c>
       <c r="F5" t="n">
-        <v>0.78</v>
+        <v>0.77</v>
       </c>
       <c r="G5" t="n">
-        <v>-455</v>
+        <v>495</v>
       </c>
       <c r="H5" t="n">
-        <v>-162185</v>
+        <v>-161820</v>
       </c>
       <c r="I5" t="n">
-        <v>-2055</v>
+        <v>-495</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -6404,28 +6434,28 @@
         <v>136</v>
       </c>
       <c r="B6" t="n">
-        <v>11794876</v>
+        <v>11927549</v>
       </c>
       <c r="C6" t="n">
-        <v>53.41</v>
+        <v>53.82</v>
       </c>
       <c r="D6" t="n">
-        <v>-343275</v>
+        <v>185372</v>
       </c>
       <c r="E6" t="n">
-        <v>10573664</v>
+        <v>10468690</v>
       </c>
       <c r="F6" t="n">
-        <v>47.88</v>
+        <v>47.24</v>
       </c>
       <c r="G6" t="n">
-        <v>-45071</v>
+        <v>-168498</v>
       </c>
       <c r="H6" t="n">
-        <v>1221212</v>
+        <v>1458859</v>
       </c>
       <c r="I6" t="n">
-        <v>-298204</v>
+        <v>353870</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -6433,28 +6463,28 @@
         <v>137</v>
       </c>
       <c r="B7" t="n">
-        <v>11794876</v>
+        <v>11927549</v>
       </c>
       <c r="C7" t="n">
-        <v>53.41</v>
+        <v>53.82</v>
       </c>
       <c r="D7" t="n">
-        <v>-343275</v>
+        <v>185372</v>
       </c>
       <c r="E7" t="n">
-        <v>10573664</v>
+        <v>10468690</v>
       </c>
       <c r="F7" t="n">
-        <v>47.88</v>
+        <v>47.24</v>
       </c>
       <c r="G7" t="n">
-        <v>-45071</v>
+        <v>-168498</v>
       </c>
       <c r="H7" t="n">
-        <v>1221212</v>
+        <v>1458859</v>
       </c>
       <c r="I7" t="n">
-        <v>-298204</v>
+        <v>353870</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -6462,28 +6492,28 @@
         <v>138</v>
       </c>
       <c r="B8" t="n">
-        <v>4203823</v>
+        <v>4372051</v>
       </c>
       <c r="C8" t="n">
-        <v>19.03</v>
+        <v>19.72</v>
       </c>
       <c r="D8" t="n">
-        <v>3186</v>
+        <v>149006</v>
       </c>
       <c r="E8" t="n">
-        <v>4711054</v>
+        <v>4763359</v>
       </c>
       <c r="F8" t="n">
-        <v>21.33</v>
+        <v>21.49</v>
       </c>
       <c r="G8" t="n">
-        <v>-81983</v>
+        <v>64929</v>
       </c>
       <c r="H8" t="n">
-        <v>-507231</v>
+        <v>-391308</v>
       </c>
       <c r="I8" t="n">
-        <v>85169</v>
+        <v>84077</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -6491,28 +6521,28 @@
         <v>139</v>
       </c>
       <c r="B9" t="n">
-        <v>20033</v>
+        <v>25626</v>
       </c>
       <c r="C9" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="D9" t="n">
+        <v>573</v>
+      </c>
+      <c r="E9" t="n">
+        <v>20951</v>
+      </c>
+      <c r="F9" t="n">
         <v>0.09</v>
       </c>
-      <c r="D9" t="n">
-        <v>1145</v>
-      </c>
-      <c r="E9" t="n">
-        <v>18449</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.08</v>
-      </c>
       <c r="G9" t="n">
-        <v>-518</v>
+        <v>-66</v>
       </c>
       <c r="H9" t="n">
-        <v>1584</v>
+        <v>4675</v>
       </c>
       <c r="I9" t="n">
-        <v>1663</v>
+        <v>639</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -6520,28 +6550,28 @@
         <v>140</v>
       </c>
       <c r="B10" t="n">
-        <v>19025</v>
+        <v>20500</v>
       </c>
       <c r="C10" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="D10" t="n">
-        <v>-85</v>
+        <v>1275</v>
       </c>
       <c r="E10" t="n">
-        <v>4650</v>
+        <v>6530</v>
       </c>
       <c r="F10" t="n">
         <v>0.02</v>
       </c>
       <c r="G10" t="n">
-        <v>190</v>
+        <v>2075</v>
       </c>
       <c r="H10" t="n">
-        <v>14375</v>
+        <v>13970</v>
       </c>
       <c r="I10" t="n">
-        <v>-275</v>
+        <v>-800</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -6549,22 +6579,22 @@
         <v>141</v>
       </c>
       <c r="B11" t="n">
-        <v>22079949</v>
+        <v>22160358</v>
       </c>
       <c r="C11" t="n">
         <v>100</v>
       </c>
       <c r="D11" t="n">
-        <v>-301349</v>
+        <v>10381</v>
       </c>
       <c r="E11" t="n">
-        <v>22079949</v>
+        <v>22160358</v>
       </c>
       <c r="F11" t="n">
         <v>100</v>
       </c>
       <c r="G11" t="n">
-        <v>-301349</v>
+        <v>10381</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -6584,15 +6614,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="5" min="5" style="35" width="10.140625"/>
+    <col customWidth="1" max="5" min="5" style="33" width="10.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -6616,8 +6646,8 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="22" t="n">
-        <v>0.4583333333333333</v>
+      <c r="A2" s="35" t="n">
+        <v>0.3333333333333333</v>
       </c>
       <c r="B2" t="s">
         <v>148</v>
@@ -6625,60 +6655,77 @@
       <c r="C2" t="s">
         <v>149</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="35" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="22" t="n"/>
-      <c r="D3" s="22" t="n"/>
-      <c r="E3" s="33" t="n"/>
-      <c r="F3" s="22" t="n"/>
+      <c r="A3" s="35" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="B3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="22" t="n"/>
-      <c r="D4" s="22" t="n"/>
-      <c r="E4" s="34" t="n"/>
-      <c r="F4" s="22" t="n"/>
+      <c r="A4" s="35" t="n"/>
+      <c r="D4" s="35" t="n"/>
+      <c r="E4" s="32" t="n"/>
+      <c r="F4" s="35" t="n"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="22" t="n"/>
-      <c r="D5" s="22" t="n"/>
-      <c r="E5" s="33" t="n"/>
-      <c r="F5" s="22" t="n"/>
+      <c r="A5" s="35" t="n"/>
+      <c r="D5" s="35" t="n"/>
+      <c r="E5" s="32" t="n"/>
+      <c r="F5" s="35" t="n"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="22" t="n"/>
-      <c r="D6" s="22" t="n"/>
-      <c r="E6" s="32" t="n"/>
-      <c r="F6" s="22" t="n"/>
+      <c r="A6" s="35" t="n"/>
+      <c r="D6" s="35" t="n"/>
+      <c r="E6" s="31" t="n"/>
+      <c r="F6" s="35" t="n"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="22" t="n"/>
-      <c r="D7" s="22" t="n"/>
-      <c r="E7" s="32" t="n"/>
-      <c r="F7" s="22" t="n"/>
+      <c r="A7" s="35" t="n"/>
+      <c r="D7" s="35" t="n"/>
+      <c r="E7" s="31" t="n"/>
+      <c r="F7" s="35" t="n"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="22" t="n"/>
-      <c r="D8" s="22" t="n"/>
-      <c r="E8" s="32" t="n"/>
-      <c r="F8" s="22" t="n"/>
+      <c r="A8" s="35" t="n"/>
+      <c r="D8" s="35" t="n"/>
+      <c r="E8" s="30" t="n"/>
+      <c r="F8" s="35" t="n"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="19" t="n"/>
-      <c r="D9" s="19" t="n"/>
-      <c r="E9" s="23" t="n"/>
-      <c r="F9" s="22" t="n"/>
+      <c r="A9" s="35" t="n"/>
+      <c r="D9" s="35" t="n"/>
+      <c r="E9" s="30" t="n"/>
+      <c r="F9" s="35" t="n"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="19" t="n"/>
+      <c r="D10" s="19" t="n"/>
+      <c r="E10" s="21" t="n"/>
+      <c r="F10" s="35" t="n"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="19" t="n"/>
@@ -6691,6 +6738,9 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="19" t="n"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="19" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>